<commit_message>
WIP of E-85 Cranking optimisation (better start at 8°c validated) cranking in xls and applied only in  v1.06 mazda-edit uk-evolve version
</commit_message>
<xml_diff>
--- a/E85Blend calculator.xlsx
+++ b/E85Blend calculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOW\RX8-E85-Vtune\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7AF243-5E1A-4DBD-BF68-E8EDF83DF20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC08350-49AF-4AD4-9F92-93814A72DB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Gasoline</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>SP95</t>
-  </si>
-  <si>
-    <t>Addition</t>
-  </si>
-  <si>
-    <t>E85</t>
   </si>
   <si>
     <t>Temp</t>
@@ -92,10 +86,10 @@
     <t>Mixture SP/E85 Volume</t>
   </si>
   <si>
-    <t>Fine tuning Addition</t>
+    <t>E85 Cranking WIP</t>
   </si>
   <si>
-    <t>E85 Cranking WIP</t>
+    <t>Fine tuning Addition</t>
   </si>
 </sst>
 </file>
@@ -157,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +185,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,12 +236,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,13 +879,13 @@
         <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -925,7 +925,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5">
         <v>0.75</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
@@ -944,7 +944,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3"/>
       <c r="E7" s="3">
@@ -956,16 +956,16 @@
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <f>(B5*B3+(1-B5)*B2)</f>
         <v>10.425000000000001</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <f>(B5*D3+(1-B5)*D2)</f>
         <v>8.15625</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <f>($E$6*D8+$E$7*$D$2)/60</f>
         <v>8.15625</v>
       </c>
@@ -974,34 +974,34 @@
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <f>B8/B2</f>
         <v>0.70918367346938782</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <f>D8/$D$2</f>
         <v>0.73979591836734704</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <f>E8/$D$2</f>
         <v>0.73979591836734704</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="12">
+      <c r="A10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11">
         <f>1+(1-B9)</f>
         <v>1.2908163265306123</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <f>1+(1-D9)</f>
         <v>1.260204081632653</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <f>1+(1-E9)</f>
         <v>1.260204081632653</v>
       </c>
@@ -2157,1481 +2157,1481 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="14">
+      <c r="A1" s="13">
         <f>'VE-Origine'!A1*1.3</f>
         <v>1.4105000000000001</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="13">
         <f>'VE-Origine'!B1*1.3</f>
         <v>1.4105000000000001</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="13">
         <f>'VE-Origine'!C1*1.3</f>
         <v>1.3793</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="13">
         <f>'VE-Origine'!D1*1.3</f>
         <v>1.3988</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="13">
         <f>'VE-Origine'!E1*1.3</f>
         <v>1.3558999999999999</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="13">
         <f>'VE-Origine'!F1*1.3</f>
         <v>1.3429</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="13">
         <f>'VE-Origine'!G1*1.3</f>
         <v>1.3714999999999999</v>
       </c>
-      <c r="H1" s="14">
+      <c r="H1" s="13">
         <f>'VE-Origine'!H1*1.3</f>
         <v>1.3728</v>
       </c>
-      <c r="I1" s="14">
+      <c r="I1" s="13">
         <f>'VE-Origine'!I1*1.3</f>
         <v>1.3052000000000001</v>
       </c>
-      <c r="J1" s="14">
+      <c r="J1" s="13">
         <f>'VE-Origine'!J1*1.3</f>
         <v>1.2706200000000001</v>
       </c>
-      <c r="K1" s="14">
+      <c r="K1" s="13">
         <f>'VE-Origine'!K1*1.3</f>
         <v>1.2547599999999999</v>
       </c>
-      <c r="L1" s="14">
+      <c r="L1" s="13">
         <f>'VE-Origine'!L1*1.3</f>
         <v>1.3298999999999999</v>
       </c>
-      <c r="M1" s="14">
+      <c r="M1" s="13">
         <f>'VE-Origine'!M1*1.3</f>
         <v>1.4430000000000003</v>
       </c>
-      <c r="N1" s="14">
+      <c r="N1" s="13">
         <f>'VE-Origine'!N1*1.3</f>
         <v>1.2967500000000001</v>
       </c>
-      <c r="O1" s="14">
+      <c r="O1" s="13">
         <f>'VE-Origine'!O1*1.3</f>
         <v>1.3038999999999998</v>
       </c>
-      <c r="P1" s="14">
+      <c r="P1" s="13">
         <f>'VE-Origine'!P1*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="Q1" s="14">
+      <c r="Q1" s="13">
         <f>'VE-Origine'!Q1*1.3</f>
         <v>1.3078000000000001</v>
       </c>
-      <c r="R1" s="14">
+      <c r="R1" s="13">
         <f>'VE-Origine'!R1*1.3</f>
         <v>1.3260000000000001</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="13">
         <f>'VE-Origine'!A2*1.3</f>
         <v>1.4105000000000001</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <f>'VE-Origine'!B2*1.3</f>
         <v>1.4105000000000001</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="13">
         <f>'VE-Origine'!C2*1.3</f>
         <v>1.3845000000000001</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <f>'VE-Origine'!D2*1.3</f>
         <v>1.3325</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <f>'VE-Origine'!E2*1.3</f>
         <v>1.3260000000000001</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="13">
         <f>'VE-Origine'!F2*1.3</f>
         <v>1.3442000000000001</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="13">
         <f>'VE-Origine'!G2*1.3</f>
         <v>1.3546</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="13">
         <f>'VE-Origine'!H2*1.3</f>
         <v>1.3351</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="13">
         <f>'VE-Origine'!I2*1.3</f>
         <v>1.2584</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="13">
         <f>'VE-Origine'!J2*1.3</f>
         <v>1.26776</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="13">
         <f>'VE-Origine'!K2*1.3</f>
         <v>1.25814</v>
       </c>
-      <c r="L2" s="14">
+      <c r="L2" s="13">
         <f>'VE-Origine'!L2*1.3</f>
         <v>1.3468</v>
       </c>
-      <c r="M2" s="14">
+      <c r="M2" s="13">
         <f>'VE-Origine'!M2*1.3</f>
         <v>1.4430000000000003</v>
       </c>
-      <c r="N2" s="14">
+      <c r="N2" s="13">
         <f>'VE-Origine'!N2*1.3</f>
         <v>1.2967500000000001</v>
       </c>
-      <c r="O2" s="14">
+      <c r="O2" s="13">
         <f>'VE-Origine'!O2*1.3</f>
         <v>1.3038999999999998</v>
       </c>
-      <c r="P2" s="14">
+      <c r="P2" s="13">
         <f>'VE-Origine'!P2*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="Q2" s="14">
+      <c r="Q2" s="13">
         <f>'VE-Origine'!Q2*1.3</f>
         <v>1.3078000000000001</v>
       </c>
-      <c r="R2" s="14">
+      <c r="R2" s="13">
         <f>'VE-Origine'!R2*1.3</f>
         <v>1.3260000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="13">
         <f>'VE-Origine'!A3*1.3</f>
         <v>1.3871</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <f>'VE-Origine'!B3*1.3</f>
         <v>1.3871</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="13">
         <f>'VE-Origine'!C3*1.3</f>
         <v>1.3793</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <f>'VE-Origine'!D3*1.3</f>
         <v>1.3220999999999998</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <f>'VE-Origine'!E3*1.3</f>
         <v>1.3182</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <f>'VE-Origine'!F3*1.3</f>
         <v>1.3272999999999999</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <f>'VE-Origine'!G3*1.3</f>
         <v>1.3546</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <f>'VE-Origine'!H3*1.3</f>
         <v>1.3234000000000001</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="13">
         <f>'VE-Origine'!I3*1.3</f>
         <v>1.2616500000000002</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="13">
         <f>'VE-Origine'!J3*1.3</f>
         <v>1.2647699999999999</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="13">
         <f>'VE-Origine'!K3*1.3</f>
         <v>1.2615200000000002</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="13">
         <f>'VE-Origine'!L3*1.3</f>
         <v>1.3650000000000002</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="13">
         <f>'VE-Origine'!M3*1.3</f>
         <v>1.3728</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="13">
         <f>'VE-Origine'!N3*1.3</f>
         <v>1.2967500000000001</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="13">
         <f>'VE-Origine'!O3*1.3</f>
         <v>1.3038999999999998</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="13">
         <f>'VE-Origine'!P3*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="Q3" s="14">
+      <c r="Q3" s="13">
         <f>'VE-Origine'!Q3*1.3</f>
         <v>1.3078000000000001</v>
       </c>
-      <c r="R3" s="14">
+      <c r="R3" s="13">
         <f>'VE-Origine'!R3*1.3</f>
         <v>1.3260000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="13">
         <f>'VE-Origine'!A4*1.3</f>
         <v>1.3858000000000001</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <f>'VE-Origine'!B4*1.3</f>
         <v>1.3858000000000001</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="13">
         <f>'VE-Origine'!C4*1.3</f>
         <v>1.3442000000000001</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <f>'VE-Origine'!D4*1.3</f>
         <v>1.3090999999999999</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <f>'VE-Origine'!E4*1.3</f>
         <v>1.3065</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <f>'VE-Origine'!F4*1.3</f>
         <v>1.3234000000000001</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <f>'VE-Origine'!G4*1.3</f>
         <v>1.3208</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <f>'VE-Origine'!H4*1.3</f>
         <v>1.3012999999999999</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="13">
         <f>'VE-Origine'!I4*1.3</f>
         <v>1.2743899999999999</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <f>'VE-Origine'!J4*1.3</f>
         <v>1.2468299999999999</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <f>'VE-Origine'!K4*1.3</f>
         <v>1.2556700000000001</v>
       </c>
-      <c r="L4" s="14">
+      <c r="L4" s="13">
         <f>'VE-Origine'!L4*1.3</f>
         <v>1.3351</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="13">
         <f>'VE-Origine'!M4*1.3</f>
         <v>1.3012999999999999</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="13">
         <f>'VE-Origine'!N4*1.3</f>
         <v>1.3429</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="13">
         <f>'VE-Origine'!O4*1.3</f>
         <v>1.3156000000000001</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="13">
         <f>'VE-Origine'!P4*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="Q4" s="13">
         <f>'VE-Origine'!Q4*1.3</f>
         <v>1.2935000000000001</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="13">
         <f>'VE-Origine'!R4*1.3</f>
         <v>1.3</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <f>'VE-Origine'!A5*1.3</f>
         <v>1.3793</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <f>'VE-Origine'!B5*1.3</f>
         <v>1.3793</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <f>'VE-Origine'!C5*1.3</f>
         <v>1.3286</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <f>'VE-Origine'!D5*1.3</f>
         <v>1.2994800000000002</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <f>'VE-Origine'!E5*1.3</f>
         <v>1.2760800000000001</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <f>'VE-Origine'!F5*1.3</f>
         <v>1.3104</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <f>'VE-Origine'!G5*1.3</f>
         <v>1.2797200000000002</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <f>'VE-Origine'!H5*1.3</f>
         <v>1.2849200000000001</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="13">
         <f>'VE-Origine'!I5*1.3</f>
         <v>1.26919</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <f>'VE-Origine'!J5*1.3</f>
         <v>1.22902</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="13">
         <f>'VE-Origine'!K5*1.3</f>
         <v>1.2655500000000002</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <f>'VE-Origine'!L5*1.3</f>
         <v>1.28427</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="13">
         <f>'VE-Origine'!M5*1.3</f>
         <v>1.3130000000000002</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="13">
         <f>'VE-Origine'!N5*1.3</f>
         <v>1.3689</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="13">
         <f>'VE-Origine'!O5*1.3</f>
         <v>1.3194999999999999</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="13">
         <f>'VE-Origine'!P5*1.3</f>
         <v>1.2935000000000001</v>
       </c>
-      <c r="Q5" s="14">
+      <c r="Q5" s="13">
         <f>'VE-Origine'!Q5*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="R5" s="14">
+      <c r="R5" s="13">
         <f>'VE-Origine'!R5*1.3</f>
         <v>1.2805</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <f>'VE-Origine'!A6*1.3</f>
         <v>1.3767</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <f>'VE-Origine'!B6*1.3</f>
         <v>1.3767</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <f>'VE-Origine'!C6*1.3</f>
         <v>1.3026</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <f>'VE-Origine'!D6*1.3</f>
         <v>1.2720500000000001</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <f>'VE-Origine'!E6*1.3</f>
         <v>1.2658100000000001</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <f>'VE-Origine'!F6*1.3</f>
         <v>1.28505</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <f>'VE-Origine'!G6*1.3</f>
         <v>1.25983</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <f>'VE-Origine'!H6*1.3</f>
         <v>1.2561900000000001</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
         <f>'VE-Origine'!I6*1.3</f>
         <v>1.2641200000000001</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <f>'VE-Origine'!J6*1.3</f>
         <v>1.2381200000000001</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <f>'VE-Origine'!K6*1.3</f>
         <v>1.2348699999999999</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <f>'VE-Origine'!L6*1.3</f>
         <v>1.3220999999999998</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="13">
         <f>'VE-Origine'!M6*1.3</f>
         <v>1.3376999999999999</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="13">
         <f>'VE-Origine'!N6*1.3</f>
         <v>1.3714999999999999</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="13">
         <f>'VE-Origine'!O6*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="13">
         <f>'VE-Origine'!P6*1.3</f>
         <v>1.2896000000000001</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="Q6" s="13">
         <f>'VE-Origine'!Q6*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6" s="13">
         <f>'VE-Origine'!R6*1.3</f>
         <v>1.3325</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <f>'VE-Origine'!A7*1.3</f>
         <v>1.3754000000000002</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <f>'VE-Origine'!B7*1.3</f>
         <v>1.3754000000000002</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <f>'VE-Origine'!C7*1.3</f>
         <v>1.2958400000000001</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <f>'VE-Origine'!D7*1.3</f>
         <v>1.2625599999999999</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <f>'VE-Origine'!E7*1.3</f>
         <v>1.2628200000000001</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <f>'VE-Origine'!F7*1.3</f>
         <v>1.26698</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <f>'VE-Origine'!G7*1.3</f>
         <v>1.2548900000000001</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <f>'VE-Origine'!H7*1.3</f>
         <v>1.2275900000000002</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="13">
         <f>'VE-Origine'!I7*1.3</f>
         <v>1.24644</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="13">
         <f>'VE-Origine'!J7*1.3</f>
         <v>1.2356500000000001</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="13">
         <f>'VE-Origine'!K7*1.3</f>
         <v>1.2169300000000001</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L7" s="13">
         <f>'VE-Origine'!L7*1.3</f>
         <v>1.3260000000000001</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="13">
         <f>'VE-Origine'!M7*1.3</f>
         <v>1.3194999999999999</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="13">
         <f>'VE-Origine'!N7*1.3</f>
         <v>1.3390000000000002</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="13">
         <f>'VE-Origine'!O7*1.3</f>
         <v>1.2792000000000001</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="13">
         <f>'VE-Origine'!P7*1.3</f>
         <v>1.3130000000000002</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="Q7" s="13">
         <f>'VE-Origine'!Q7*1.3</f>
         <v>1.2908999999999999</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R7" s="13">
         <f>'VE-Origine'!R7*1.3</f>
         <v>1.3130000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <f>'VE-Origine'!A8*1.3</f>
         <v>1.3442000000000001</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <f>'VE-Origine'!B8*1.3</f>
         <v>1.3442000000000001</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <f>'VE-Origine'!C8*1.3</f>
         <v>1.27712</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <f>'VE-Origine'!D8*1.3</f>
         <v>1.2687999999999999</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <f>'VE-Origine'!E8*1.3</f>
         <v>1.26711</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <f>'VE-Origine'!F8*1.3</f>
         <v>1.25502</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <f>'VE-Origine'!G8*1.3</f>
         <v>1.24735</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <f>'VE-Origine'!H8*1.3</f>
         <v>1.2421500000000001</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="13">
         <f>'VE-Origine'!I8*1.3</f>
         <v>1.23123</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="13">
         <f>'VE-Origine'!J8*1.3</f>
         <v>1.21641</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="13">
         <f>'VE-Origine'!K8*1.3</f>
         <v>1.2753000000000001</v>
       </c>
-      <c r="L8" s="14">
+      <c r="L8" s="13">
         <f>'VE-Origine'!L8*1.3</f>
         <v>1.3208</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="13">
         <f>'VE-Origine'!M8*1.3</f>
         <v>1.3065</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="13">
         <f>'VE-Origine'!N8*1.3</f>
         <v>1.2967500000000001</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="13">
         <f>'VE-Origine'!O8*1.3</f>
         <v>1.3130000000000002</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="13">
         <f>'VE-Origine'!P8*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="Q8" s="14">
+      <c r="Q8" s="13">
         <f>'VE-Origine'!Q8*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="R8" s="14">
+      <c r="R8" s="13">
         <f>'VE-Origine'!R8*1.3</f>
         <v>1.3</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="13">
         <f>'VE-Origine'!A9*1.3</f>
         <v>1.3130000000000002</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <f>'VE-Origine'!B9*1.3</f>
         <v>1.3130000000000002</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <f>'VE-Origine'!C9*1.3</f>
         <v>1.2584</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <f>'VE-Origine'!D9*1.3</f>
         <v>1.2496900000000002</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <f>'VE-Origine'!E9*1.3</f>
         <v>1.27868</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <f>'VE-Origine'!F9*1.3</f>
         <v>1.25515</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <f>'VE-Origine'!G9*1.3</f>
         <v>1.23994</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <f>'VE-Origine'!H9*1.3</f>
         <v>1.2378600000000002</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="13">
         <f>'VE-Origine'!I9*1.3</f>
         <v>1.22187</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="13">
         <f>'VE-Origine'!J9*1.3</f>
         <v>1.27504</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="13">
         <f>'VE-Origine'!K9*1.3</f>
         <v>1.2805</v>
       </c>
-      <c r="L9" s="14">
+      <c r="L9" s="13">
         <f>'VE-Origine'!L9*1.3</f>
         <v>1.3052000000000001</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="13">
         <f>'VE-Origine'!M9*1.3</f>
         <v>1.2935000000000001</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="13">
         <f>'VE-Origine'!N9*1.3</f>
         <v>1.3494000000000002</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9" s="13">
         <f>'VE-Origine'!O9*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="13">
         <f>'VE-Origine'!P9*1.3</f>
         <v>1.3052000000000001</v>
       </c>
-      <c r="Q9" s="14">
+      <c r="Q9" s="13">
         <f>'VE-Origine'!Q9*1.3</f>
         <v>1.2844</v>
       </c>
-      <c r="R9" s="14">
+      <c r="R9" s="13">
         <f>'VE-Origine'!R9*1.3</f>
         <v>1.274</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
+      <c r="A10" s="13">
         <f>'VE-Origine'!A10*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="13">
         <f>'VE-Origine'!B10*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <f>'VE-Origine'!C10*1.3</f>
         <v>1.2647699999999999</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <f>'VE-Origine'!D10*1.3</f>
         <v>1.23071</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <f>'VE-Origine'!E10*1.3</f>
         <v>1.25684</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <f>'VE-Origine'!F10*1.3</f>
         <v>1.2298</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <f>'VE-Origine'!G10*1.3</f>
         <v>1.2435800000000001</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <f>'VE-Origine'!H10*1.3</f>
         <v>1.23214</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="13">
         <f>'VE-Origine'!I10*1.3</f>
         <v>1.24098</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <f>'VE-Origine'!J10*1.3</f>
         <v>1.2522900000000001</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="13">
         <f>'VE-Origine'!K10*1.3</f>
         <v>1.2918100000000001</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="13">
         <f>'VE-Origine'!L10*1.3</f>
         <v>1.2902500000000001</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="13">
         <f>'VE-Origine'!M10*1.3</f>
         <v>1.2935000000000001</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="13">
         <f>'VE-Origine'!N10*1.3</f>
         <v>1.3298999999999999</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10" s="13">
         <f>'VE-Origine'!O10*1.3</f>
         <v>1.2896000000000001</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="13">
         <f>'VE-Origine'!P10*1.3</f>
         <v>1.2779</v>
       </c>
-      <c r="Q10" s="14">
+      <c r="Q10" s="13">
         <f>'VE-Origine'!Q10*1.3</f>
         <v>1.2687999999999999</v>
       </c>
-      <c r="R10" s="14">
+      <c r="R10" s="13">
         <f>'VE-Origine'!R10*1.3</f>
         <v>1.2609999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <f>'VE-Origine'!A11*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <f>'VE-Origine'!B11*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <f>'VE-Origine'!C11*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <f>'VE-Origine'!D11*1.3</f>
         <v>1.2299300000000002</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <f>'VE-Origine'!E11*1.3</f>
         <v>1.2349999999999999</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <f>'VE-Origine'!F11*1.3</f>
         <v>1.20458</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <f>'VE-Origine'!G11*1.3</f>
         <v>1.21628</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <f>'VE-Origine'!H11*1.3</f>
         <v>1.22109</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="13">
         <f>'VE-Origine'!I11*1.3</f>
         <v>1.2421500000000001</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="13">
         <f>'VE-Origine'!J11*1.3</f>
         <v>1.26633</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="13">
         <f>'VE-Origine'!K11*1.3</f>
         <v>1.3038999999999998</v>
       </c>
-      <c r="L11" s="14">
+      <c r="L11" s="13">
         <f>'VE-Origine'!L11*1.3</f>
         <v>1.2609999999999999</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="13">
         <f>'VE-Origine'!M11*1.3</f>
         <v>1.2967500000000001</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="13">
         <f>'VE-Origine'!N11*1.3</f>
         <v>1.2967500000000001</v>
       </c>
-      <c r="O11" s="14">
+      <c r="O11" s="13">
         <f>'VE-Origine'!O11*1.3</f>
         <v>1.2805</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="13">
         <f>'VE-Origine'!P11*1.3</f>
         <v>1.2935000000000001</v>
       </c>
-      <c r="Q11" s="14">
+      <c r="Q11" s="13">
         <f>'VE-Origine'!Q11*1.3</f>
         <v>1.274</v>
       </c>
-      <c r="R11" s="14">
+      <c r="R11" s="13">
         <f>'VE-Origine'!R11*1.3</f>
         <v>1.2609999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <f>'VE-Origine'!A12*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <f>'VE-Origine'!B12*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="13">
         <f>'VE-Origine'!C12*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <f>'VE-Origine'!D12*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <f>'VE-Origine'!E12*1.3</f>
         <v>1.1830000000000001</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <f>'VE-Origine'!F12*1.3</f>
         <v>1.2025000000000001</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <f>'VE-Origine'!G12*1.3</f>
         <v>1.19093</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <f>'VE-Origine'!H12*1.3</f>
         <v>1.2074400000000001</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="13">
         <f>'VE-Origine'!I12*1.3</f>
         <v>1.2197900000000002</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="13">
         <f>'VE-Origine'!J12*1.3</f>
         <v>1.2805</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="13">
         <f>'VE-Origine'!K12*1.3</f>
         <v>1.2837500000000002</v>
       </c>
-      <c r="L12" s="14">
+      <c r="L12" s="13">
         <f>'VE-Origine'!L12*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="13">
         <f>'VE-Origine'!M12*1.3</f>
         <v>1.2805</v>
       </c>
-      <c r="N12" s="14">
+      <c r="N12" s="13">
         <f>'VE-Origine'!N12*1.3</f>
         <v>1.27725</v>
       </c>
-      <c r="O12" s="14">
+      <c r="O12" s="13">
         <f>'VE-Origine'!O12*1.3</f>
         <v>1.2609999999999999</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="13">
         <f>'VE-Origine'!P12*1.3</f>
         <v>1.2844</v>
       </c>
-      <c r="Q12" s="14">
+      <c r="Q12" s="13">
         <f>'VE-Origine'!Q12*1.3</f>
         <v>1.2609999999999999</v>
       </c>
-      <c r="R12" s="14">
+      <c r="R12" s="13">
         <f>'VE-Origine'!R12*1.3</f>
         <v>1.2349999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <f>'VE-Origine'!A13*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="13">
         <f>'VE-Origine'!B13*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <f>'VE-Origine'!C13*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <f>'VE-Origine'!D13*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <f>'VE-Origine'!E13*1.3</f>
         <v>1.1830000000000001</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="13">
         <f>'VE-Origine'!F13*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <f>'VE-Origine'!G13*1.3</f>
         <v>1.1550499999999999</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="13">
         <f>'VE-Origine'!H13*1.3</f>
         <v>1.1869000000000001</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="13">
         <f>'VE-Origine'!I13*1.3</f>
         <v>1.2119900000000001</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="13">
         <f>'VE-Origine'!J13*1.3</f>
         <v>1.3038999999999998</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="13">
         <f>'VE-Origine'!K13*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="L13" s="14">
+      <c r="L13" s="13">
         <f>'VE-Origine'!L13*1.3</f>
         <v>1.27725</v>
       </c>
-      <c r="M13" s="14">
+      <c r="M13" s="13">
         <f>'VE-Origine'!M13*1.3</f>
         <v>1.2642500000000001</v>
       </c>
-      <c r="N13" s="14">
+      <c r="N13" s="13">
         <f>'VE-Origine'!N13*1.3</f>
         <v>1.2609999999999999</v>
       </c>
-      <c r="O13" s="14">
+      <c r="O13" s="13">
         <f>'VE-Origine'!O13*1.3</f>
         <v>1.248</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="13">
         <f>'VE-Origine'!P13*1.3</f>
         <v>1.2687999999999999</v>
       </c>
-      <c r="Q13" s="14">
+      <c r="Q13" s="13">
         <f>'VE-Origine'!Q13*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="R13" s="14">
+      <c r="R13" s="13">
         <f>'VE-Origine'!R13*1.3</f>
         <v>1.2505999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <f>'VE-Origine'!A14*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <f>'VE-Origine'!B14*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <f>'VE-Origine'!C14*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <f>'VE-Origine'!D14*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <f>'VE-Origine'!E14*1.3</f>
         <v>1.1830000000000001</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="13">
         <f>'VE-Origine'!F14*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <f>'VE-Origine'!G14*1.3</f>
         <v>1.1811799999999999</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="13">
         <f>'VE-Origine'!H14*1.3</f>
         <v>1.21875</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <f>'VE-Origine'!I14*1.3</f>
         <v>1.274</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="13">
         <f>'VE-Origine'!J14*1.3</f>
         <v>1.2805</v>
       </c>
-      <c r="K14" s="14">
+      <c r="K14" s="13">
         <f>'VE-Origine'!K14*1.3</f>
         <v>1.2675000000000001</v>
       </c>
-      <c r="L14" s="14">
+      <c r="L14" s="13">
         <f>'VE-Origine'!L14*1.3</f>
         <v>1.2609999999999999</v>
       </c>
-      <c r="M14" s="14">
+      <c r="M14" s="13">
         <f>'VE-Origine'!M14*1.3</f>
         <v>1.2382500000000001</v>
       </c>
-      <c r="N14" s="14">
+      <c r="N14" s="13">
         <f>'VE-Origine'!N14*1.3</f>
         <v>1.2642500000000001</v>
       </c>
-      <c r="O14" s="14">
+      <c r="O14" s="13">
         <f>'VE-Origine'!O14*1.3</f>
         <v>1.248</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="13">
         <f>'VE-Origine'!P14*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="Q14" s="13">
         <f>'VE-Origine'!Q14*1.3</f>
         <v>1.2701</v>
       </c>
-      <c r="R14" s="14">
+      <c r="R14" s="13">
         <f>'VE-Origine'!R14*1.3</f>
         <v>1.274</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <f>'VE-Origine'!A15*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="13">
         <f>'VE-Origine'!B15*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="13">
         <f>'VE-Origine'!C15*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <f>'VE-Origine'!D15*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="13">
         <f>'VE-Origine'!E15*1.3</f>
         <v>1.1830000000000001</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="13">
         <f>'VE-Origine'!F15*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="13">
         <f>'VE-Origine'!G15*1.3</f>
         <v>1.1811799999999999</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="13">
         <f>'VE-Origine'!H15*1.3</f>
         <v>1.21875</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="13">
         <f>'VE-Origine'!I15*1.3</f>
         <v>1.274</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="13">
         <f>'VE-Origine'!J15*1.3</f>
         <v>1.25346</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="13">
         <f>'VE-Origine'!K15*1.3</f>
         <v>1.2675000000000001</v>
       </c>
-      <c r="L15" s="14">
+      <c r="L15" s="13">
         <f>'VE-Origine'!L15*1.3</f>
         <v>1.2561900000000001</v>
       </c>
-      <c r="M15" s="14">
+      <c r="M15" s="13">
         <f>'VE-Origine'!M15*1.3</f>
         <v>1.2287600000000001</v>
       </c>
-      <c r="N15" s="14">
+      <c r="N15" s="13">
         <f>'VE-Origine'!N15*1.3</f>
         <v>1.2594400000000001</v>
       </c>
-      <c r="O15" s="14">
+      <c r="O15" s="13">
         <f>'VE-Origine'!O15*1.3</f>
         <v>1.2698400000000001</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="13">
         <f>'VE-Origine'!P15*1.3</f>
         <v>1.3</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="Q15" s="13">
         <f>'VE-Origine'!Q15*1.3</f>
         <v>1.2701</v>
       </c>
-      <c r="R15" s="14">
+      <c r="R15" s="13">
         <f>'VE-Origine'!R15*1.3</f>
         <v>1.1653199999999999</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <f>'VE-Origine'!A16*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="13">
         <f>'VE-Origine'!B16*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="13">
         <f>'VE-Origine'!C16*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <f>'VE-Origine'!D16*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <f>'VE-Origine'!E16*1.3</f>
         <v>1.1830000000000001</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <f>'VE-Origine'!F16*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <f>'VE-Origine'!G16*1.3</f>
         <v>1.1811799999999999</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="13">
         <f>'VE-Origine'!H16*1.3</f>
         <v>1.21875</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="13">
         <f>'VE-Origine'!I16*1.3</f>
         <v>1.274</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <f>'VE-Origine'!J16*1.3</f>
         <v>1.2521599999999999</v>
       </c>
-      <c r="K16" s="14">
+      <c r="K16" s="13">
         <f>'VE-Origine'!K16*1.3</f>
         <v>1.23604</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="13">
         <f>'VE-Origine'!L16*1.3</f>
         <v>1.2544999999999999</v>
       </c>
-      <c r="M16" s="14">
+      <c r="M16" s="13">
         <f>'VE-Origine'!M16*1.3</f>
         <v>1.22525</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16" s="13">
         <f>'VE-Origine'!N16*1.3</f>
         <v>1.2454000000000001</v>
       </c>
-      <c r="O16" s="14">
+      <c r="O16" s="13">
         <f>'VE-Origine'!O16*1.3</f>
         <v>1.2779</v>
       </c>
-      <c r="P16" s="14">
+      <c r="P16" s="13">
         <f>'VE-Origine'!P16*1.3</f>
         <v>1.25905</v>
       </c>
-      <c r="Q16" s="14">
+      <c r="Q16" s="13">
         <f>'VE-Origine'!Q16*1.3</f>
         <v>1.2196600000000002</v>
       </c>
-      <c r="R16" s="14">
+      <c r="R16" s="13">
         <f>'VE-Origine'!R16*1.3</f>
         <v>1.16259</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="14">
+      <c r="A17" s="13">
         <f>'VE-Origine'!A17*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="13">
         <f>'VE-Origine'!B17*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="13">
         <f>'VE-Origine'!C17*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="13">
         <f>'VE-Origine'!D17*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <f>'VE-Origine'!E17*1.3</f>
         <v>1.1830000000000001</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <f>'VE-Origine'!F17*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <f>'VE-Origine'!G17*1.3</f>
         <v>1.1811799999999999</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="13">
         <f>'VE-Origine'!H17*1.3</f>
         <v>1.21875</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="13">
         <f>'VE-Origine'!I17*1.3</f>
         <v>1.274</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="13">
         <f>'VE-Origine'!J17*1.3</f>
         <v>1.2507299999999999</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="13">
         <f>'VE-Origine'!K17*1.3</f>
         <v>1.2025000000000001</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="13">
         <f>'VE-Origine'!L17*1.3</f>
         <v>1.2355200000000002</v>
       </c>
-      <c r="M17" s="14">
+      <c r="M17" s="13">
         <f>'VE-Origine'!M17*1.3</f>
         <v>1.20627</v>
       </c>
-      <c r="N17" s="14">
+      <c r="N17" s="13">
         <f>'VE-Origine'!N17*1.3</f>
         <v>1.23045</v>
       </c>
-      <c r="O17" s="14">
+      <c r="O17" s="13">
         <f>'VE-Origine'!O17*1.3</f>
         <v>1.2779</v>
       </c>
-      <c r="P17" s="14">
+      <c r="P17" s="13">
         <f>'VE-Origine'!P17*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="Q17" s="14">
+      <c r="Q17" s="13">
         <f>'VE-Origine'!Q17*1.3</f>
         <v>1.1661000000000001</v>
       </c>
-      <c r="R17" s="14">
+      <c r="R17" s="13">
         <f>'VE-Origine'!R17*1.3</f>
         <v>1.1598600000000001</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="A18" s="13">
         <f>'VE-Origine'!A18*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="13">
         <f>'VE-Origine'!B18*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="13">
         <f>'VE-Origine'!C18*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <f>'VE-Origine'!D18*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <f>'VE-Origine'!E18*1.3</f>
         <v>1.1830000000000001</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="13">
         <f>'VE-Origine'!F18*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <f>'VE-Origine'!G18*1.3</f>
         <v>1.1811799999999999</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="13">
         <f>'VE-Origine'!H18*1.3</f>
         <v>1.21875</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="13">
         <f>'VE-Origine'!I18*1.3</f>
         <v>1.274</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="13">
         <f>'VE-Origine'!J18*1.3</f>
         <v>1.24735</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="13">
         <f>'VE-Origine'!K18*1.3</f>
         <v>1.1939200000000001</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="13">
         <f>'VE-Origine'!L18*1.3</f>
         <v>1.1900200000000001</v>
       </c>
-      <c r="M18" s="14">
+      <c r="M18" s="13">
         <f>'VE-Origine'!M18*1.3</f>
         <v>1.1607700000000001</v>
       </c>
-      <c r="N18" s="14">
+      <c r="N18" s="13">
         <f>'VE-Origine'!N18*1.3</f>
         <v>1.1947000000000001</v>
       </c>
-      <c r="O18" s="14">
+      <c r="O18" s="13">
         <f>'VE-Origine'!O18*1.3</f>
         <v>1.2129000000000001</v>
       </c>
-      <c r="P18" s="14">
+      <c r="P18" s="13">
         <f>'VE-Origine'!P18*1.3</f>
         <v>1.20692</v>
       </c>
-      <c r="Q18" s="14">
+      <c r="Q18" s="13">
         <f>'VE-Origine'!Q18*1.3</f>
         <v>1.1575200000000001</v>
       </c>
-      <c r="R18" s="14">
+      <c r="R18" s="13">
         <f>'VE-Origine'!R18*1.3</f>
         <v>1.1529700000000001</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="A19" s="13">
         <f>'VE-Origine'!A19*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="13">
         <f>'VE-Origine'!B19*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="13">
         <f>'VE-Origine'!C19*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="13">
         <f>'VE-Origine'!D19*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <f>'VE-Origine'!E19*1.3</f>
         <v>1.1830000000000001</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="13">
         <f>'VE-Origine'!F19*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <f>'VE-Origine'!G19*1.3</f>
         <v>1.1811799999999999</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="13">
         <f>'VE-Origine'!H19*1.3</f>
         <v>1.21875</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I19" s="13">
         <f>'VE-Origine'!I19*1.3</f>
         <v>1.274</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="13">
         <f>'VE-Origine'!J19*1.3</f>
         <v>1.2404600000000001</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="13">
         <f>'VE-Origine'!K19*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L19" s="13">
         <f>'VE-Origine'!L19*1.3</f>
         <v>1.17442</v>
       </c>
-      <c r="M19" s="14">
+      <c r="M19" s="13">
         <f>'VE-Origine'!M19*1.3</f>
         <v>1.14517</v>
       </c>
-      <c r="N19" s="14">
+      <c r="N19" s="13">
         <f>'VE-Origine'!N19*1.3</f>
         <v>1.1791</v>
       </c>
-      <c r="O19" s="14">
+      <c r="O19" s="13">
         <f>'VE-Origine'!O19*1.3</f>
         <v>1.1973</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P19" s="13">
         <f>'VE-Origine'!P19*1.3</f>
         <v>1.1895</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="Q19" s="13">
         <f>'VE-Origine'!Q19*1.3</f>
         <v>1.1401000000000001</v>
       </c>
-      <c r="R19" s="14">
+      <c r="R19" s="13">
         <f>'VE-Origine'!R19*1.3</f>
         <v>1.1393199999999999</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
+      <c r="A20" s="13">
         <f>'VE-Origine'!A20*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="13">
         <f>'VE-Origine'!B20*1.3</f>
         <v>1.2869999999999999</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="13">
         <f>'VE-Origine'!C20*1.3</f>
         <v>1.2415</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="13">
         <f>'VE-Origine'!D20*1.3</f>
         <v>1.2155</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <f>'VE-Origine'!E20*1.3</f>
         <v>1.1830000000000001</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="13">
         <f>'VE-Origine'!F20*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <f>'VE-Origine'!G20*1.3</f>
         <v>1.1811799999999999</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <f>'VE-Origine'!H20*1.3</f>
         <v>1.21875</v>
       </c>
-      <c r="I20" s="14">
+      <c r="I20" s="13">
         <f>'VE-Origine'!I20*1.3</f>
         <v>1.274</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="13">
         <f>'VE-Origine'!J20*1.3</f>
         <v>1.2404600000000001</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="13">
         <f>'VE-Origine'!K20*1.3</f>
         <v>1.1765000000000001</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L20" s="13">
         <f>'VE-Origine'!L20*1.3</f>
         <v>1.1640200000000001</v>
       </c>
-      <c r="M20" s="14">
+      <c r="M20" s="13">
         <f>'VE-Origine'!M20*1.3</f>
         <v>1.1347700000000001</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N20" s="13">
         <f>'VE-Origine'!N20*1.3</f>
         <v>1.1687000000000001</v>
       </c>
-      <c r="O20" s="14">
+      <c r="O20" s="13">
         <f>'VE-Origine'!O20*1.3</f>
         <v>1.1869000000000001</v>
       </c>
-      <c r="P20" s="14">
+      <c r="P20" s="13">
         <f>'VE-Origine'!P20*1.3</f>
         <v>1.1895</v>
       </c>
-      <c r="Q20" s="14">
+      <c r="Q20" s="13">
         <f>'VE-Origine'!Q20*1.3</f>
         <v>1.1401000000000001</v>
       </c>
-      <c r="R20" s="14">
+      <c r="R20" s="13">
         <f>'VE-Origine'!R20*1.3</f>
         <v>1.1393199999999999</v>
       </c>
@@ -6633,20 +6633,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC026DA-F509-4385-B6B3-72E60872EBDC}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="8">
         <v>-30</v>
@@ -6746,231 +6746,116 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="9">
+        <v>15</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="G3" s="14">
         <v>0.5</v>
       </c>
-      <c r="C3" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="9">
+      <c r="H3" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="I3" s="14">
         <v>0.1</v>
       </c>
-      <c r="H3" s="9">
+      <c r="J3" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="14">
         <v>0</v>
       </c>
-      <c r="I3" s="9">
+      <c r="M3" s="14">
         <v>0</v>
       </c>
-      <c r="J3" s="9">
+      <c r="N3" s="14">
         <v>0</v>
       </c>
-      <c r="K3" s="9">
+      <c r="O3" s="14">
         <v>0</v>
       </c>
-      <c r="L3" s="9">
-        <v>0</v>
-      </c>
-      <c r="M3" s="9">
-        <v>0</v>
-      </c>
-      <c r="N3" s="9">
-        <v>0</v>
-      </c>
-      <c r="O3" s="9">
-        <v>0</v>
-      </c>
-      <c r="P3" s="9">
+      <c r="P3" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9">
+        <f t="shared" ref="B4:E4" si="0">IF(B2+B2*B3&lt;130,B2+B2*B3,130)</f>
+        <v>130</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>78.75</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="F4" s="9">
+        <f>IF(F2+F2*F3&lt;130,F2+F2*F3,130)</f>
+        <v>61.25</v>
+      </c>
+      <c r="G4" s="9">
+        <f>IF(G2+G2*G3&lt;130,G2+G2*G3,130)</f>
+        <v>52.5</v>
+      </c>
+      <c r="H4" s="9">
+        <f>IF(H2+H2*H3&lt;130,H2+H2*H3,130)</f>
+        <v>43.75</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="shared" ref="I4:P4" si="1">IF(I2+I2*I3&lt;130,I2+I2*I3,130)</f>
+        <v>38.5</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" si="1"/>
+        <v>38.5</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="1"/>
+        <v>9.9</v>
+      </c>
+      <c r="L4" s="9">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B4" s="10">
-        <f>IF(B2+B2*B3&lt;130,B2+B2*B3,130)</f>
-        <v>130</v>
-      </c>
-      <c r="C4" s="10">
-        <f t="shared" ref="C4:P4" si="0">IF(C2+C2*C3&lt;130,C2+C2*C3,130)</f>
-        <v>91.26</v>
-      </c>
-      <c r="D4" s="10">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="E4" s="10">
-        <f t="shared" si="0"/>
-        <v>45.5</v>
-      </c>
-      <c r="F4" s="10">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="G4" s="10">
-        <f t="shared" si="0"/>
-        <v>38.5</v>
-      </c>
-      <c r="H4" s="10">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="I4" s="10">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="J4" s="10">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="K4" s="10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="L4" s="10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M4" s="10">
-        <f t="shared" si="0"/>
+      <c r="M4" s="9">
+        <f t="shared" si="1"/>
         <v>5.2480000000000002</v>
       </c>
-      <c r="N4" s="10">
-        <f t="shared" si="0"/>
+      <c r="N4" s="9">
+        <f t="shared" si="1"/>
         <v>3.1440000000000001</v>
       </c>
-      <c r="O4" s="10">
-        <f t="shared" si="0"/>
+      <c r="O4" s="9">
+        <f t="shared" si="1"/>
         <v>3.1440000000000001</v>
       </c>
-      <c r="P4" s="10">
-        <f t="shared" si="0"/>
-        <v>3.1440000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="9">
-        <v>5</v>
-      </c>
-      <c r="C5" s="9">
-        <v>5</v>
-      </c>
-      <c r="D5" s="9">
-        <v>5</v>
-      </c>
-      <c r="E5" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="F5" s="9">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="H5" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="I5" s="9">
-        <v>0.125</v>
-      </c>
-      <c r="J5" s="9">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0</v>
-      </c>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="9">
-        <v>0</v>
-      </c>
-      <c r="N5" s="9">
-        <v>0</v>
-      </c>
-      <c r="O5" s="9">
-        <v>0</v>
-      </c>
-      <c r="P5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="10">
-        <f>IF(B2+B2*B5&lt;130,B2+B2*B5,130)</f>
-        <v>130</v>
-      </c>
-      <c r="C6" s="10">
-        <f>IF(C2+C2*C5&lt;130,C2+C2*C5,130)</f>
-        <v>130</v>
-      </c>
-      <c r="D6" s="10">
-        <f>IF(D2+D2*D5&lt;130,D2+D2*D5,130)</f>
-        <v>130</v>
-      </c>
-      <c r="E6" s="10">
-        <f>IF(E2+E2*E5&lt;130,E2+E2*E5,130)</f>
-        <v>122.5</v>
-      </c>
-      <c r="F6" s="10">
-        <f>IF(F2+F2*F5&lt;130,F2+F2*F5,130)</f>
-        <v>70</v>
-      </c>
-      <c r="G6" s="10">
-        <f>IF(G2+G2*G5&lt;130,G2+G2*G5,130)</f>
-        <v>52.5</v>
-      </c>
-      <c r="H6" s="10">
-        <f>IF(H2+H2*H5&lt;130,H2+H2*H5,130)</f>
-        <v>43.75</v>
-      </c>
-      <c r="I6" s="10">
-        <f>IF(I2+I2*I5&lt;130,I2+I2*I5,130)</f>
-        <v>39.375</v>
-      </c>
-      <c r="J6" s="10">
-        <f>IF(J2+J2*J5&lt;130,J2+J2*J5,130)</f>
-        <v>35</v>
-      </c>
-      <c r="K6" s="10">
-        <f>IF(K2+K2*K5&lt;130,K2+K2*K5,130)</f>
-        <v>9</v>
-      </c>
-      <c r="L6" s="10">
-        <f>IF(L2+L2*L5&lt;130,L2+L2*L5,130)</f>
-        <v>8</v>
-      </c>
-      <c r="M6" s="10">
-        <f>IF(M2+M2*M5&lt;130,M2+M2*M5,130)</f>
-        <v>5.2480000000000002</v>
-      </c>
-      <c r="N6" s="10">
-        <f>IF(N2+N2*N5&lt;130,N2+N2*N5,130)</f>
-        <v>3.1440000000000001</v>
-      </c>
-      <c r="O6" s="10">
-        <f>IF(O2+O2*O5&lt;130,O2+O2*O5,130)</f>
-        <v>3.1440000000000001</v>
-      </c>
-      <c r="P6" s="10">
-        <f>IF(P2+P2*P5&lt;130,P2+P2*P5,130)</f>
+      <c r="P4" s="9">
+        <f t="shared" si="1"/>
         <v>3.1440000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cold Cranking Addtion decrease + change warmup RPM limitation 4k RPM until 57 deg celsius
</commit_message>
<xml_diff>
--- a/E85Blend calculator.xlsx
+++ b/E85Blend calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOW\RX8-E85-Vtune\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8234E8E1-511B-49F5-8E8C-729B0B92F986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE554989-423A-4F70-8A47-7FC2BCF56FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
   </bookViews>
   <sheets>
     <sheet name="Blend" sheetId="1" r:id="rId1"/>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C507529D-A20D-4ABB-AAE4-BE6AA5385A82}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6532,7 +6532,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8027,7 +8027,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection sqref="A1:R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9522,7 +9522,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R20"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11016,8 +11016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC026DA-F509-4385-B6B3-72E60872EBDC}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11136,43 +11136,43 @@
         <v>1.5</v>
       </c>
       <c r="D3" s="14">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="E3" s="14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F3" s="14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G3" s="14">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H3" s="14">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="I3" s="14">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J3" s="14">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="K3" s="14">
         <v>0.1</v>
       </c>
       <c r="L3" s="14">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M3" s="14">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="N3" s="14">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="14">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="14">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -11189,31 +11189,31 @@
       </c>
       <c r="D4" s="9">
         <f t="shared" si="0"/>
-        <v>87.5</v>
+        <v>78.75</v>
       </c>
       <c r="E4" s="9">
         <f t="shared" si="0"/>
-        <v>87.5</v>
+        <v>70</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>52.5</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>43.75</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>38.5</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>38.5</v>
       </c>
       <c r="J4" s="9">
         <f t="shared" si="0"/>
-        <v>52.5</v>
+        <v>38.5</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" si="0"/>
@@ -11221,23 +11221,23 @@
       </c>
       <c r="L4" s="9">
         <f t="shared" si="0"/>
-        <v>8.8000000000000007</v>
+        <v>8</v>
       </c>
       <c r="M4" s="9">
         <f t="shared" si="0"/>
-        <v>5.7728000000000002</v>
+        <v>5.2480000000000002</v>
       </c>
       <c r="N4" s="9">
         <f t="shared" si="0"/>
-        <v>3.4584000000000001</v>
+        <v>3.1440000000000001</v>
       </c>
       <c r="O4" s="9">
         <f t="shared" si="0"/>
-        <v>3.4584000000000001</v>
+        <v>3.1440000000000001</v>
       </c>
       <c r="P4" s="9">
         <f t="shared" si="0"/>
-        <v>3.4584000000000001</v>
+        <v>3.1440000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -11250,7 +11250,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I24:I25"/>
+      <selection sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
1.07 Update and tested over 1K KM
</commit_message>
<xml_diff>
--- a/E85Blend calculator.xlsx
+++ b/E85Blend calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOW\RX8-E85-Vtune\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE554989-423A-4F70-8A47-7FC2BCF56FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB8F6BF-D982-407D-A0A1-7ADC45AE0020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
   </bookViews>
   <sheets>
     <sheet name="Blend" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,15 @@
     <sheet name="VE-E85-theory" sheetId="6" r:id="rId3"/>
     <sheet name="VE-E85" sheetId="3" r:id="rId4"/>
     <sheet name="VE-Mix" sheetId="5" r:id="rId5"/>
-    <sheet name="Cranking" sheetId="4" r:id="rId6"/>
-    <sheet name="DWELL Stock" sheetId="10" r:id="rId7"/>
-    <sheet name="DWELL RRP4" sheetId="11" r:id="rId8"/>
-    <sheet name="Oil Injector Load " sheetId="12" r:id="rId9"/>
-    <sheet name="Oil Injector Throttle" sheetId="13" r:id="rId10"/>
-    <sheet name="AFR 1 (RX8 Evolve 2006 UK)" sheetId="7" r:id="rId11"/>
-    <sheet name="AFR 2 (RX8 Evolve 2006 UK)" sheetId="8" r:id="rId12"/>
-    <sheet name="AFR 3 (RX8 Evolve 2006 UK)" sheetId="9" r:id="rId13"/>
+    <sheet name="Injectors Sizing" sheetId="14" r:id="rId6"/>
+    <sheet name="Cranking" sheetId="4" r:id="rId7"/>
+    <sheet name="DWELL Stock" sheetId="10" r:id="rId8"/>
+    <sheet name="DWELL RRP4" sheetId="11" r:id="rId9"/>
+    <sheet name="Oil Injector Load " sheetId="12" r:id="rId10"/>
+    <sheet name="Oil Injector Throttle" sheetId="13" r:id="rId11"/>
+    <sheet name="AFR 1 (RX8 Evolve 2006 UK)" sheetId="7" r:id="rId12"/>
+    <sheet name="AFR 2 (RX8 Evolve 2006 UK)" sheetId="8" r:id="rId13"/>
+    <sheet name="AFR 3 (RX8 Evolve 2006 UK)" sheetId="9" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Gasoline</t>
   </si>
@@ -94,6 +95,27 @@
   </si>
   <si>
     <t>Fine tuning Addition</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Injector Scaling 1</t>
+  </si>
+  <si>
+    <t>Injector Scaling 2</t>
+  </si>
+  <si>
+    <t>Injector Scaling 3</t>
+  </si>
+  <si>
+    <t>E-85</t>
+  </si>
+  <si>
+    <t>Kindzi Map</t>
+  </si>
+  <si>
+    <t>Multiply By 2 - 1/4 of total</t>
   </si>
 </sst>
 </file>
@@ -155,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +226,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -232,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -253,6 +281,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C507529D-A20D-4ABB-AAE4-BE6AA5385A82}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,6 +1053,1024 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97B2FC1-B655-492A-B49E-5A9630364CB0}">
+  <dimension ref="A1:S17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="8">
+        <v>3</v>
+      </c>
+      <c r="B1" s="8">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8">
+        <v>3</v>
+      </c>
+      <c r="G1" s="8">
+        <v>3</v>
+      </c>
+      <c r="H1" s="8">
+        <v>3</v>
+      </c>
+      <c r="I1" s="8">
+        <v>3</v>
+      </c>
+      <c r="J1" s="8">
+        <v>5</v>
+      </c>
+      <c r="K1" s="8">
+        <v>7</v>
+      </c>
+      <c r="L1" s="8">
+        <v>7</v>
+      </c>
+      <c r="M1" s="8">
+        <v>7</v>
+      </c>
+      <c r="N1" s="8">
+        <v>11</v>
+      </c>
+      <c r="O1" s="8">
+        <v>12</v>
+      </c>
+      <c r="P1" s="8">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="8">
+        <v>19</v>
+      </c>
+      <c r="R1" s="8">
+        <v>19</v>
+      </c>
+      <c r="S1" s="8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8">
+        <v>3</v>
+      </c>
+      <c r="G2" s="8">
+        <v>3</v>
+      </c>
+      <c r="H2" s="8">
+        <v>3</v>
+      </c>
+      <c r="I2" s="8">
+        <v>3</v>
+      </c>
+      <c r="J2" s="8">
+        <v>5</v>
+      </c>
+      <c r="K2" s="8">
+        <v>7</v>
+      </c>
+      <c r="L2" s="8">
+        <v>7</v>
+      </c>
+      <c r="M2" s="8">
+        <v>7</v>
+      </c>
+      <c r="N2" s="8">
+        <v>11</v>
+      </c>
+      <c r="O2" s="8">
+        <v>15</v>
+      </c>
+      <c r="P2" s="8">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>20</v>
+      </c>
+      <c r="R2" s="8">
+        <v>21</v>
+      </c>
+      <c r="S2" s="8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>3</v>
+      </c>
+      <c r="B3" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3" s="8">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8">
+        <v>3</v>
+      </c>
+      <c r="G3" s="8">
+        <v>3</v>
+      </c>
+      <c r="H3" s="8">
+        <v>3</v>
+      </c>
+      <c r="I3" s="8">
+        <v>3</v>
+      </c>
+      <c r="J3" s="8">
+        <v>5</v>
+      </c>
+      <c r="K3" s="8">
+        <v>7</v>
+      </c>
+      <c r="L3" s="8">
+        <v>7</v>
+      </c>
+      <c r="M3" s="8">
+        <v>7</v>
+      </c>
+      <c r="N3" s="8">
+        <v>11</v>
+      </c>
+      <c r="O3" s="8">
+        <v>17</v>
+      </c>
+      <c r="P3" s="8">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>21</v>
+      </c>
+      <c r="R3" s="8">
+        <v>22</v>
+      </c>
+      <c r="S3" s="8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>3</v>
+      </c>
+      <c r="G4" s="8">
+        <v>3</v>
+      </c>
+      <c r="H4" s="8">
+        <v>3</v>
+      </c>
+      <c r="I4" s="8">
+        <v>3</v>
+      </c>
+      <c r="J4" s="8">
+        <v>5</v>
+      </c>
+      <c r="K4" s="8">
+        <v>7</v>
+      </c>
+      <c r="L4" s="8">
+        <v>7</v>
+      </c>
+      <c r="M4" s="8">
+        <v>7</v>
+      </c>
+      <c r="N4" s="8">
+        <v>11</v>
+      </c>
+      <c r="O4" s="8">
+        <v>18</v>
+      </c>
+      <c r="P4" s="8">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>22</v>
+      </c>
+      <c r="R4" s="8">
+        <v>23</v>
+      </c>
+      <c r="S4" s="8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8">
+        <v>3</v>
+      </c>
+      <c r="G5" s="8">
+        <v>3</v>
+      </c>
+      <c r="H5" s="8">
+        <v>4</v>
+      </c>
+      <c r="I5" s="8">
+        <v>5</v>
+      </c>
+      <c r="J5" s="8">
+        <v>6</v>
+      </c>
+      <c r="K5" s="8">
+        <v>8</v>
+      </c>
+      <c r="L5" s="8">
+        <v>7</v>
+      </c>
+      <c r="M5" s="8">
+        <v>9</v>
+      </c>
+      <c r="N5" s="8">
+        <v>12</v>
+      </c>
+      <c r="O5" s="8">
+        <v>18</v>
+      </c>
+      <c r="P5" s="8">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>23</v>
+      </c>
+      <c r="R5" s="8">
+        <v>45</v>
+      </c>
+      <c r="S5" s="8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>6</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8">
+        <v>3</v>
+      </c>
+      <c r="G6" s="8">
+        <v>3</v>
+      </c>
+      <c r="H6" s="8">
+        <v>5</v>
+      </c>
+      <c r="I6" s="8">
+        <v>6</v>
+      </c>
+      <c r="J6" s="8">
+        <v>9</v>
+      </c>
+      <c r="K6" s="8">
+        <v>10</v>
+      </c>
+      <c r="L6" s="8">
+        <v>11</v>
+      </c>
+      <c r="M6" s="8">
+        <v>12</v>
+      </c>
+      <c r="N6" s="8">
+        <v>15</v>
+      </c>
+      <c r="O6" s="8">
+        <v>21</v>
+      </c>
+      <c r="P6" s="8">
+        <v>23</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>45</v>
+      </c>
+      <c r="R6" s="8">
+        <v>45</v>
+      </c>
+      <c r="S6" s="8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8">
+        <v>9</v>
+      </c>
+      <c r="E7" s="8">
+        <v>6</v>
+      </c>
+      <c r="F7" s="8">
+        <v>5</v>
+      </c>
+      <c r="G7" s="8">
+        <v>8</v>
+      </c>
+      <c r="H7" s="8">
+        <v>8</v>
+      </c>
+      <c r="I7" s="8">
+        <v>8</v>
+      </c>
+      <c r="J7" s="8">
+        <v>11</v>
+      </c>
+      <c r="K7" s="8">
+        <v>13</v>
+      </c>
+      <c r="L7" s="8">
+        <v>14</v>
+      </c>
+      <c r="M7" s="8">
+        <v>16</v>
+      </c>
+      <c r="N7" s="8">
+        <v>19</v>
+      </c>
+      <c r="O7" s="8">
+        <v>23</v>
+      </c>
+      <c r="P7" s="8">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>45</v>
+      </c>
+      <c r="R7" s="8">
+        <v>45</v>
+      </c>
+      <c r="S7" s="8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8">
+        <v>19</v>
+      </c>
+      <c r="C8" s="8">
+        <v>19</v>
+      </c>
+      <c r="D8" s="8">
+        <v>16</v>
+      </c>
+      <c r="E8" s="8">
+        <v>16</v>
+      </c>
+      <c r="F8" s="8">
+        <v>16</v>
+      </c>
+      <c r="G8" s="8">
+        <v>19</v>
+      </c>
+      <c r="H8" s="8">
+        <v>16</v>
+      </c>
+      <c r="I8" s="8">
+        <v>14</v>
+      </c>
+      <c r="J8" s="8">
+        <v>13</v>
+      </c>
+      <c r="K8" s="8">
+        <v>15</v>
+      </c>
+      <c r="L8" s="8">
+        <v>17</v>
+      </c>
+      <c r="M8" s="8">
+        <v>17</v>
+      </c>
+      <c r="N8" s="8">
+        <v>20</v>
+      </c>
+      <c r="O8" s="8">
+        <v>45</v>
+      </c>
+      <c r="P8" s="8">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>45</v>
+      </c>
+      <c r="R8" s="8">
+        <v>45</v>
+      </c>
+      <c r="S8" s="8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>3</v>
+      </c>
+      <c r="B9" s="8">
+        <v>19</v>
+      </c>
+      <c r="C9" s="8">
+        <v>19</v>
+      </c>
+      <c r="D9" s="8">
+        <v>16</v>
+      </c>
+      <c r="E9" s="8">
+        <v>16</v>
+      </c>
+      <c r="F9" s="8">
+        <v>16</v>
+      </c>
+      <c r="G9" s="8">
+        <v>19</v>
+      </c>
+      <c r="H9" s="8">
+        <v>16</v>
+      </c>
+      <c r="I9" s="8">
+        <v>14</v>
+      </c>
+      <c r="J9" s="8">
+        <v>15</v>
+      </c>
+      <c r="K9" s="8">
+        <v>18</v>
+      </c>
+      <c r="L9" s="8">
+        <v>19</v>
+      </c>
+      <c r="M9" s="8">
+        <v>19</v>
+      </c>
+      <c r="N9" s="8">
+        <v>20</v>
+      </c>
+      <c r="O9" s="8">
+        <v>45</v>
+      </c>
+      <c r="P9" s="8">
+        <v>45</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>45</v>
+      </c>
+      <c r="R9" s="8">
+        <v>45</v>
+      </c>
+      <c r="S9" s="8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8">
+        <v>19</v>
+      </c>
+      <c r="D10" s="8">
+        <v>16</v>
+      </c>
+      <c r="E10" s="8">
+        <v>16</v>
+      </c>
+      <c r="F10" s="8">
+        <v>16</v>
+      </c>
+      <c r="G10" s="8">
+        <v>19</v>
+      </c>
+      <c r="H10" s="8">
+        <v>17</v>
+      </c>
+      <c r="I10" s="8">
+        <v>16</v>
+      </c>
+      <c r="J10" s="8">
+        <v>17</v>
+      </c>
+      <c r="K10" s="8">
+        <v>20</v>
+      </c>
+      <c r="L10" s="8">
+        <v>20</v>
+      </c>
+      <c r="M10" s="8">
+        <v>20</v>
+      </c>
+      <c r="N10" s="8">
+        <v>21</v>
+      </c>
+      <c r="O10" s="8">
+        <v>45</v>
+      </c>
+      <c r="P10" s="8">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>45</v>
+      </c>
+      <c r="R10" s="8">
+        <v>48</v>
+      </c>
+      <c r="S10" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8">
+        <v>17</v>
+      </c>
+      <c r="F11" s="8">
+        <v>16</v>
+      </c>
+      <c r="G11" s="8">
+        <v>19</v>
+      </c>
+      <c r="H11" s="8">
+        <v>18</v>
+      </c>
+      <c r="I11" s="8">
+        <v>19</v>
+      </c>
+      <c r="J11" s="8">
+        <v>20</v>
+      </c>
+      <c r="K11" s="8">
+        <v>20</v>
+      </c>
+      <c r="L11" s="8">
+        <v>21</v>
+      </c>
+      <c r="M11" s="8">
+        <v>21</v>
+      </c>
+      <c r="N11" s="8">
+        <v>21</v>
+      </c>
+      <c r="O11" s="8">
+        <v>45</v>
+      </c>
+      <c r="P11" s="8">
+        <v>45</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>47</v>
+      </c>
+      <c r="R11" s="8">
+        <v>49</v>
+      </c>
+      <c r="S11" s="8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8">
+        <v>21</v>
+      </c>
+      <c r="C12" s="8">
+        <v>21</v>
+      </c>
+      <c r="D12" s="8">
+        <v>21</v>
+      </c>
+      <c r="E12" s="8">
+        <v>20</v>
+      </c>
+      <c r="F12" s="8">
+        <v>19</v>
+      </c>
+      <c r="G12" s="8">
+        <v>20</v>
+      </c>
+      <c r="H12" s="8">
+        <v>21</v>
+      </c>
+      <c r="I12" s="8">
+        <v>22</v>
+      </c>
+      <c r="J12" s="8">
+        <v>22</v>
+      </c>
+      <c r="K12" s="8">
+        <v>22</v>
+      </c>
+      <c r="L12" s="8">
+        <v>22</v>
+      </c>
+      <c r="M12" s="8">
+        <v>22</v>
+      </c>
+      <c r="N12" s="8">
+        <v>22</v>
+      </c>
+      <c r="O12" s="8">
+        <v>46</v>
+      </c>
+      <c r="P12" s="8">
+        <v>47</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>50</v>
+      </c>
+      <c r="R12" s="8">
+        <v>53</v>
+      </c>
+      <c r="S12" s="8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>3</v>
+      </c>
+      <c r="B13" s="8">
+        <v>21</v>
+      </c>
+      <c r="C13" s="8">
+        <v>21</v>
+      </c>
+      <c r="D13" s="8">
+        <v>22</v>
+      </c>
+      <c r="E13" s="8">
+        <v>22</v>
+      </c>
+      <c r="F13" s="8">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8">
+        <v>22</v>
+      </c>
+      <c r="H13" s="8">
+        <v>22</v>
+      </c>
+      <c r="I13" s="8">
+        <v>26</v>
+      </c>
+      <c r="J13" s="8">
+        <v>26</v>
+      </c>
+      <c r="K13" s="8">
+        <v>26</v>
+      </c>
+      <c r="L13" s="8">
+        <v>26</v>
+      </c>
+      <c r="M13" s="8">
+        <v>26</v>
+      </c>
+      <c r="N13" s="8">
+        <v>46</v>
+      </c>
+      <c r="O13" s="8">
+        <v>46</v>
+      </c>
+      <c r="P13" s="8">
+        <v>47</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>52</v>
+      </c>
+      <c r="R13" s="8">
+        <v>56</v>
+      </c>
+      <c r="S13" s="8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>3</v>
+      </c>
+      <c r="B14" s="8">
+        <v>21</v>
+      </c>
+      <c r="C14" s="8">
+        <v>21</v>
+      </c>
+      <c r="D14" s="8">
+        <v>22</v>
+      </c>
+      <c r="E14" s="8">
+        <v>22</v>
+      </c>
+      <c r="F14" s="8">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8">
+        <v>22</v>
+      </c>
+      <c r="H14" s="8">
+        <v>22</v>
+      </c>
+      <c r="I14" s="8">
+        <v>27</v>
+      </c>
+      <c r="J14" s="8">
+        <v>27</v>
+      </c>
+      <c r="K14" s="8">
+        <v>27</v>
+      </c>
+      <c r="L14" s="8">
+        <v>27</v>
+      </c>
+      <c r="M14" s="8">
+        <v>27</v>
+      </c>
+      <c r="N14" s="8">
+        <v>46</v>
+      </c>
+      <c r="O14" s="8">
+        <v>46</v>
+      </c>
+      <c r="P14" s="8">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>54</v>
+      </c>
+      <c r="R14" s="8">
+        <v>58</v>
+      </c>
+      <c r="S14" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>3</v>
+      </c>
+      <c r="B15" s="8">
+        <v>21</v>
+      </c>
+      <c r="C15" s="8">
+        <v>21</v>
+      </c>
+      <c r="D15" s="8">
+        <v>22</v>
+      </c>
+      <c r="E15" s="8">
+        <v>23</v>
+      </c>
+      <c r="F15" s="8">
+        <v>23</v>
+      </c>
+      <c r="G15" s="8">
+        <v>22</v>
+      </c>
+      <c r="H15" s="8">
+        <v>22</v>
+      </c>
+      <c r="I15" s="8">
+        <v>27</v>
+      </c>
+      <c r="J15" s="8">
+        <v>27</v>
+      </c>
+      <c r="K15" s="8">
+        <v>28</v>
+      </c>
+      <c r="L15" s="8">
+        <v>27</v>
+      </c>
+      <c r="M15" s="8">
+        <v>46</v>
+      </c>
+      <c r="N15" s="8">
+        <v>46</v>
+      </c>
+      <c r="O15" s="8">
+        <v>48</v>
+      </c>
+      <c r="P15" s="8">
+        <v>54</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>57</v>
+      </c>
+      <c r="R15" s="8">
+        <v>60</v>
+      </c>
+      <c r="S15" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>3</v>
+      </c>
+      <c r="B16" s="8">
+        <v>21</v>
+      </c>
+      <c r="C16" s="8">
+        <v>21</v>
+      </c>
+      <c r="D16" s="8">
+        <v>22</v>
+      </c>
+      <c r="E16" s="8">
+        <v>23</v>
+      </c>
+      <c r="F16" s="8">
+        <v>23</v>
+      </c>
+      <c r="G16" s="8">
+        <v>23</v>
+      </c>
+      <c r="H16" s="8">
+        <v>23</v>
+      </c>
+      <c r="I16" s="8">
+        <v>27</v>
+      </c>
+      <c r="J16" s="8">
+        <v>28</v>
+      </c>
+      <c r="K16" s="8">
+        <v>28</v>
+      </c>
+      <c r="L16" s="8">
+        <v>46</v>
+      </c>
+      <c r="M16" s="8">
+        <v>46</v>
+      </c>
+      <c r="N16" s="8">
+        <v>46</v>
+      </c>
+      <c r="O16" s="8">
+        <v>49</v>
+      </c>
+      <c r="P16" s="8">
+        <v>55</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>57</v>
+      </c>
+      <c r="R16" s="8">
+        <v>60</v>
+      </c>
+      <c r="S16" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>3</v>
+      </c>
+      <c r="B17" s="8">
+        <v>21</v>
+      </c>
+      <c r="C17" s="8">
+        <v>21</v>
+      </c>
+      <c r="D17" s="8">
+        <v>22</v>
+      </c>
+      <c r="E17" s="8">
+        <v>23</v>
+      </c>
+      <c r="F17" s="8">
+        <v>23</v>
+      </c>
+      <c r="G17" s="8">
+        <v>23</v>
+      </c>
+      <c r="H17" s="8">
+        <v>23</v>
+      </c>
+      <c r="I17" s="8">
+        <v>27</v>
+      </c>
+      <c r="J17" s="8">
+        <v>28</v>
+      </c>
+      <c r="K17" s="8">
+        <v>28</v>
+      </c>
+      <c r="L17" s="8">
+        <v>46</v>
+      </c>
+      <c r="M17" s="8">
+        <v>46</v>
+      </c>
+      <c r="N17" s="8">
+        <v>46</v>
+      </c>
+      <c r="O17" s="8">
+        <v>60</v>
+      </c>
+      <c r="P17" s="8">
+        <v>60</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>60</v>
+      </c>
+      <c r="R17" s="8">
+        <v>60</v>
+      </c>
+      <c r="S17" s="8">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C1BFA8-FAA2-458D-BB89-D1C1BEA124CE}">
   <dimension ref="A1:S4"/>
   <sheetViews>
@@ -1273,7 +2321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FAD0D9-AE8A-4D98-80BC-EF41A6EF9C0B}">
   <dimension ref="A1:V20"/>
   <sheetViews>
@@ -2646,7 +3694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DB8ACFA-CA2F-4655-907B-0205748B0D5F}">
   <dimension ref="A1:V20"/>
   <sheetViews>
@@ -4019,7 +5067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5846CAB-E682-4DD5-91E5-D81AA5E0B943}">
   <dimension ref="A1:V20"/>
   <sheetViews>
@@ -5397,7 +6445,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8027,7 +9075,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:R20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11013,231 +12061,60 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC026DA-F509-4385-B6B3-72E60872EBDC}">
-  <dimension ref="A1:P4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4867405C-A678-47D1-9072-ADEDA89E5AE2}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:P4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="8">
-        <v>-30</v>
-      </c>
-      <c r="C1" s="8">
-        <v>-20</v>
-      </c>
-      <c r="D1" s="8">
-        <v>-10</v>
-      </c>
-      <c r="E1" s="8">
-        <v>0</v>
-      </c>
-      <c r="F1" s="8">
-        <v>10</v>
-      </c>
-      <c r="G1" s="8">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8">
-        <v>30</v>
-      </c>
-      <c r="I1" s="8">
-        <v>40</v>
-      </c>
-      <c r="J1" s="8">
-        <v>50</v>
-      </c>
-      <c r="K1" s="8">
-        <v>60</v>
-      </c>
-      <c r="L1" s="8">
-        <v>70</v>
-      </c>
-      <c r="M1" s="8">
-        <v>80</v>
-      </c>
-      <c r="N1" s="8">
-        <v>90</v>
-      </c>
-      <c r="O1" s="8">
-        <v>100</v>
-      </c>
-      <c r="P1" s="8">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
-        <v>101.8</v>
-      </c>
-      <c r="C2" s="2">
-        <v>60.84</v>
-      </c>
-      <c r="D2" s="2">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2">
-        <v>35</v>
-      </c>
-      <c r="F2" s="2">
-        <v>35</v>
-      </c>
-      <c r="G2" s="2">
-        <v>35</v>
-      </c>
-      <c r="H2" s="2">
-        <v>35</v>
-      </c>
-      <c r="I2" s="2">
-        <v>35</v>
-      </c>
-      <c r="J2" s="2">
-        <v>35</v>
-      </c>
-      <c r="K2" s="2">
-        <v>9</v>
-      </c>
-      <c r="L2" s="2">
-        <v>8</v>
-      </c>
-      <c r="M2" s="2">
-        <v>5.2480000000000002</v>
-      </c>
-      <c r="N2" s="2">
-        <v>3.1440000000000001</v>
-      </c>
-      <c r="O2" s="2">
-        <v>3.1440000000000001</v>
-      </c>
-      <c r="P2" s="2">
-        <v>3.1440000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="B2" s="16">
+        <v>369.47199999999998</v>
+      </c>
+      <c r="C2" s="1">
+        <f>B2-(B2*30%)</f>
+        <v>258.63040000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="14">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="D3" s="14">
-        <v>1.25</v>
-      </c>
-      <c r="E3" s="14">
-        <v>1</v>
-      </c>
-      <c r="F3" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="G3" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="H3" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="I3" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="J3" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="K3" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="L3" s="14">
-        <v>0</v>
-      </c>
-      <c r="M3" s="14">
-        <v>0</v>
-      </c>
-      <c r="N3" s="14">
-        <v>0</v>
-      </c>
-      <c r="O3" s="14">
-        <v>0</v>
-      </c>
-      <c r="P3" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B3" s="16">
+        <v>475.93</v>
+      </c>
+      <c r="C3" s="1">
+        <f>B3-(B3*30%)</f>
+        <v>333.15100000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="9">
-        <f>IF(B2*B3+B2&lt;130,B2*B3+B2,130)</f>
-        <v>130</v>
-      </c>
-      <c r="C4" s="9">
-        <f t="shared" ref="C4:P4" si="0">IF(C2*C3+C2&lt;130,C2*C3+C2,130)</f>
-        <v>130</v>
-      </c>
-      <c r="D4" s="9">
-        <f t="shared" si="0"/>
-        <v>78.75</v>
-      </c>
-      <c r="E4" s="9">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="F4" s="9">
-        <f t="shared" si="0"/>
-        <v>52.5</v>
-      </c>
-      <c r="G4" s="9">
-        <f t="shared" si="0"/>
-        <v>43.75</v>
-      </c>
-      <c r="H4" s="9">
-        <f t="shared" si="0"/>
-        <v>38.5</v>
-      </c>
-      <c r="I4" s="9">
-        <f t="shared" si="0"/>
-        <v>38.5</v>
-      </c>
-      <c r="J4" s="9">
-        <f t="shared" si="0"/>
-        <v>38.5</v>
-      </c>
-      <c r="K4" s="9">
-        <f t="shared" si="0"/>
-        <v>9.9</v>
-      </c>
-      <c r="L4" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="M4" s="9">
-        <f t="shared" si="0"/>
-        <v>5.2480000000000002</v>
-      </c>
-      <c r="N4" s="9">
-        <f t="shared" si="0"/>
-        <v>3.1440000000000001</v>
-      </c>
-      <c r="O4" s="9">
-        <f t="shared" si="0"/>
-        <v>3.1440000000000001</v>
-      </c>
-      <c r="P4" s="9">
-        <f t="shared" si="0"/>
-        <v>3.1440000000000001</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="16">
+        <v>475.93</v>
+      </c>
+      <c r="C4" s="1">
+        <f>B4-(B4*30%)</f>
+        <v>333.15100000000001</v>
       </c>
     </row>
   </sheetData>
@@ -11246,6 +12123,401 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC026DA-F509-4385-B6B3-72E60872EBDC}">
+  <dimension ref="A1:P9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="8">
+        <v>-30</v>
+      </c>
+      <c r="C1" s="8">
+        <v>-20</v>
+      </c>
+      <c r="D1" s="8">
+        <v>-10</v>
+      </c>
+      <c r="E1" s="8">
+        <v>0</v>
+      </c>
+      <c r="F1" s="8">
+        <v>10</v>
+      </c>
+      <c r="G1" s="8">
+        <v>20</v>
+      </c>
+      <c r="H1" s="8">
+        <v>30</v>
+      </c>
+      <c r="I1" s="8">
+        <v>40</v>
+      </c>
+      <c r="J1" s="8">
+        <v>50</v>
+      </c>
+      <c r="K1" s="8">
+        <v>60</v>
+      </c>
+      <c r="L1" s="8">
+        <v>70</v>
+      </c>
+      <c r="M1" s="8">
+        <v>80</v>
+      </c>
+      <c r="N1" s="8">
+        <v>90</v>
+      </c>
+      <c r="O1" s="8">
+        <v>100</v>
+      </c>
+      <c r="P1" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>101.8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>60.84</v>
+      </c>
+      <c r="D2" s="2">
+        <v>35</v>
+      </c>
+      <c r="E2" s="2">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2">
+        <v>35</v>
+      </c>
+      <c r="H2" s="2">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2">
+        <v>35</v>
+      </c>
+      <c r="J2" s="2">
+        <v>35</v>
+      </c>
+      <c r="K2" s="2">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2">
+        <v>8</v>
+      </c>
+      <c r="M2" s="2">
+        <v>5.2480000000000002</v>
+      </c>
+      <c r="N2" s="2">
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="O2" s="2">
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="P2" s="2">
+        <v>3.1440000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="E3" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="14">
+        <v>1</v>
+      </c>
+      <c r="G3" s="14">
+        <v>1</v>
+      </c>
+      <c r="H3" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="K3" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="14">
+        <v>0</v>
+      </c>
+      <c r="M3" s="14">
+        <v>0</v>
+      </c>
+      <c r="N3" s="14">
+        <v>0</v>
+      </c>
+      <c r="O3" s="14">
+        <v>0</v>
+      </c>
+      <c r="P3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9">
+        <f>IF(B2*B3+B2&lt;130,B2*B3+B2,130)</f>
+        <v>130</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" ref="C4:P4" si="0">IF(C2*C3+C2&lt;130,C2*C3+C2,130)</f>
+        <v>130</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="E4" s="9">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="G4" s="9">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+      <c r="J4" s="9">
+        <f t="shared" si="0"/>
+        <v>38.5</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="0"/>
+        <v>9.9</v>
+      </c>
+      <c r="L4" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M4" s="9">
+        <f t="shared" si="0"/>
+        <v>5.2480000000000002</v>
+      </c>
+      <c r="N4" s="9">
+        <f t="shared" si="0"/>
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="O4" s="9">
+        <f t="shared" si="0"/>
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="P4" s="9">
+        <f t="shared" si="0"/>
+        <v>3.1440000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <v>130</v>
+      </c>
+      <c r="C6" s="8">
+        <v>130</v>
+      </c>
+      <c r="D6" s="8">
+        <v>87.5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>87.5</v>
+      </c>
+      <c r="F6" s="8">
+        <v>70</v>
+      </c>
+      <c r="G6" s="8">
+        <v>52.5</v>
+      </c>
+      <c r="H6" s="8">
+        <v>52.5</v>
+      </c>
+      <c r="I6" s="8">
+        <v>52.5</v>
+      </c>
+      <c r="J6" s="8">
+        <v>52.5</v>
+      </c>
+      <c r="K6" s="8">
+        <v>9.8960000000000008</v>
+      </c>
+      <c r="L6" s="8">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="M6" s="8">
+        <v>5.7759999999999998</v>
+      </c>
+      <c r="N6" s="8">
+        <v>3.456</v>
+      </c>
+      <c r="O6" s="8">
+        <v>3.456</v>
+      </c>
+      <c r="P6" s="8">
+        <v>3.456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2">
+        <v>101.8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>60.84</v>
+      </c>
+      <c r="D8" s="2">
+        <v>35</v>
+      </c>
+      <c r="E8" s="2">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2">
+        <v>11</v>
+      </c>
+      <c r="J8" s="2">
+        <v>10</v>
+      </c>
+      <c r="K8" s="2">
+        <v>9</v>
+      </c>
+      <c r="L8" s="2">
+        <v>8</v>
+      </c>
+      <c r="M8" s="2">
+        <v>5.2480000000000002</v>
+      </c>
+      <c r="N8" s="2">
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="O8" s="2">
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="P8" s="2">
+        <v>3.1440000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="9">
+        <f>B8</f>
+        <v>101.8</v>
+      </c>
+      <c r="C9" s="17">
+        <f>IF(C8*2*0.75&lt;130,C8*2*0.75,130)</f>
+        <v>91.26</v>
+      </c>
+      <c r="D9" s="17">
+        <f>IF(D8*2*0.75&lt;130,D8*2*0.75,130)</f>
+        <v>52.5</v>
+      </c>
+      <c r="E9" s="17">
+        <f>IF(E8*2*0.75&lt;130,E8*2*0.75,130)</f>
+        <v>52.5</v>
+      </c>
+      <c r="F9" s="17">
+        <f>IF(F8*2*0.75&lt;130,F8*2*0.75,130)</f>
+        <v>30</v>
+      </c>
+      <c r="G9" s="17">
+        <f>IF(G8*2*0.75&lt;130,G8*2*0.75,130)</f>
+        <v>19.5</v>
+      </c>
+      <c r="H9" s="17">
+        <f>IF(H8*2*0.75&lt;130,H8*2*0.75,130)</f>
+        <v>18</v>
+      </c>
+      <c r="I9" s="17">
+        <f>IF(I8*2*0.75&lt;130,I8*2*0.75,130)</f>
+        <v>16.5</v>
+      </c>
+      <c r="J9" s="17">
+        <f>IF(J8*2*0.75&lt;130,J8*2*0.75,130)</f>
+        <v>15</v>
+      </c>
+      <c r="K9" s="9">
+        <f>K8</f>
+        <v>9</v>
+      </c>
+      <c r="L9" s="9">
+        <f>L8</f>
+        <v>8</v>
+      </c>
+      <c r="M9" s="9">
+        <f>M8</f>
+        <v>5.2480000000000002</v>
+      </c>
+      <c r="N9" s="9">
+        <f>N8</f>
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="O9" s="9">
+        <f>O8</f>
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="P9" s="9">
+        <f>P8</f>
+        <v>3.1440000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745AD7B9-4B1D-4E8C-A42C-E86EAA5F24F9}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -11521,12 +12793,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622EF6D1-D033-4A41-9B00-C212908A9BEE}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I9"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11876,1022 +13148,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97B2FC1-B655-492A-B49E-5A9630364CB0}">
-  <dimension ref="A1:S17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:S17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="8">
-        <v>3</v>
-      </c>
-      <c r="B1" s="8">
-        <v>3</v>
-      </c>
-      <c r="C1" s="8">
-        <v>3</v>
-      </c>
-      <c r="D1" s="8">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8">
-        <v>3</v>
-      </c>
-      <c r="G1" s="8">
-        <v>3</v>
-      </c>
-      <c r="H1" s="8">
-        <v>3</v>
-      </c>
-      <c r="I1" s="8">
-        <v>3</v>
-      </c>
-      <c r="J1" s="8">
-        <v>5</v>
-      </c>
-      <c r="K1" s="8">
-        <v>7</v>
-      </c>
-      <c r="L1" s="8">
-        <v>7</v>
-      </c>
-      <c r="M1" s="8">
-        <v>7</v>
-      </c>
-      <c r="N1" s="8">
-        <v>11</v>
-      </c>
-      <c r="O1" s="8">
-        <v>12</v>
-      </c>
-      <c r="P1" s="8">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="8">
-        <v>19</v>
-      </c>
-      <c r="R1" s="8">
-        <v>19</v>
-      </c>
-      <c r="S1" s="8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>3</v>
-      </c>
-      <c r="B2" s="8">
-        <v>3</v>
-      </c>
-      <c r="C2" s="8">
-        <v>3</v>
-      </c>
-      <c r="D2" s="8">
-        <v>3</v>
-      </c>
-      <c r="E2" s="8">
-        <v>3</v>
-      </c>
-      <c r="F2" s="8">
-        <v>3</v>
-      </c>
-      <c r="G2" s="8">
-        <v>3</v>
-      </c>
-      <c r="H2" s="8">
-        <v>3</v>
-      </c>
-      <c r="I2" s="8">
-        <v>3</v>
-      </c>
-      <c r="J2" s="8">
-        <v>5</v>
-      </c>
-      <c r="K2" s="8">
-        <v>7</v>
-      </c>
-      <c r="L2" s="8">
-        <v>7</v>
-      </c>
-      <c r="M2" s="8">
-        <v>7</v>
-      </c>
-      <c r="N2" s="8">
-        <v>11</v>
-      </c>
-      <c r="O2" s="8">
-        <v>15</v>
-      </c>
-      <c r="P2" s="8">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>20</v>
-      </c>
-      <c r="R2" s="8">
-        <v>21</v>
-      </c>
-      <c r="S2" s="8">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8">
-        <v>3</v>
-      </c>
-      <c r="C3" s="8">
-        <v>3</v>
-      </c>
-      <c r="D3" s="8">
-        <v>3</v>
-      </c>
-      <c r="E3" s="8">
-        <v>3</v>
-      </c>
-      <c r="F3" s="8">
-        <v>3</v>
-      </c>
-      <c r="G3" s="8">
-        <v>3</v>
-      </c>
-      <c r="H3" s="8">
-        <v>3</v>
-      </c>
-      <c r="I3" s="8">
-        <v>3</v>
-      </c>
-      <c r="J3" s="8">
-        <v>5</v>
-      </c>
-      <c r="K3" s="8">
-        <v>7</v>
-      </c>
-      <c r="L3" s="8">
-        <v>7</v>
-      </c>
-      <c r="M3" s="8">
-        <v>7</v>
-      </c>
-      <c r="N3" s="8">
-        <v>11</v>
-      </c>
-      <c r="O3" s="8">
-        <v>17</v>
-      </c>
-      <c r="P3" s="8">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>21</v>
-      </c>
-      <c r="R3" s="8">
-        <v>22</v>
-      </c>
-      <c r="S3" s="8">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8">
-        <v>3</v>
-      </c>
-      <c r="C4" s="8">
-        <v>3</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8">
-        <v>3</v>
-      </c>
-      <c r="G4" s="8">
-        <v>3</v>
-      </c>
-      <c r="H4" s="8">
-        <v>3</v>
-      </c>
-      <c r="I4" s="8">
-        <v>3</v>
-      </c>
-      <c r="J4" s="8">
-        <v>5</v>
-      </c>
-      <c r="K4" s="8">
-        <v>7</v>
-      </c>
-      <c r="L4" s="8">
-        <v>7</v>
-      </c>
-      <c r="M4" s="8">
-        <v>7</v>
-      </c>
-      <c r="N4" s="8">
-        <v>11</v>
-      </c>
-      <c r="O4" s="8">
-        <v>18</v>
-      </c>
-      <c r="P4" s="8">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>22</v>
-      </c>
-      <c r="R4" s="8">
-        <v>23</v>
-      </c>
-      <c r="S4" s="8">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8">
-        <v>3</v>
-      </c>
-      <c r="D5" s="8">
-        <v>3</v>
-      </c>
-      <c r="E5" s="8">
-        <v>3</v>
-      </c>
-      <c r="F5" s="8">
-        <v>3</v>
-      </c>
-      <c r="G5" s="8">
-        <v>3</v>
-      </c>
-      <c r="H5" s="8">
-        <v>4</v>
-      </c>
-      <c r="I5" s="8">
-        <v>5</v>
-      </c>
-      <c r="J5" s="8">
-        <v>6</v>
-      </c>
-      <c r="K5" s="8">
-        <v>8</v>
-      </c>
-      <c r="L5" s="8">
-        <v>7</v>
-      </c>
-      <c r="M5" s="8">
-        <v>9</v>
-      </c>
-      <c r="N5" s="8">
-        <v>12</v>
-      </c>
-      <c r="O5" s="8">
-        <v>18</v>
-      </c>
-      <c r="P5" s="8">
-        <v>22</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>23</v>
-      </c>
-      <c r="R5" s="8">
-        <v>45</v>
-      </c>
-      <c r="S5" s="8">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8">
-        <v>3</v>
-      </c>
-      <c r="C6" s="8">
-        <v>3</v>
-      </c>
-      <c r="D6" s="8">
-        <v>6</v>
-      </c>
-      <c r="E6" s="8">
-        <v>3</v>
-      </c>
-      <c r="F6" s="8">
-        <v>3</v>
-      </c>
-      <c r="G6" s="8">
-        <v>3</v>
-      </c>
-      <c r="H6" s="8">
-        <v>5</v>
-      </c>
-      <c r="I6" s="8">
-        <v>6</v>
-      </c>
-      <c r="J6" s="8">
-        <v>9</v>
-      </c>
-      <c r="K6" s="8">
-        <v>10</v>
-      </c>
-      <c r="L6" s="8">
-        <v>11</v>
-      </c>
-      <c r="M6" s="8">
-        <v>12</v>
-      </c>
-      <c r="N6" s="8">
-        <v>15</v>
-      </c>
-      <c r="O6" s="8">
-        <v>21</v>
-      </c>
-      <c r="P6" s="8">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="8">
-        <v>45</v>
-      </c>
-      <c r="R6" s="8">
-        <v>45</v>
-      </c>
-      <c r="S6" s="8">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>3</v>
-      </c>
-      <c r="B7" s="8">
-        <v>6</v>
-      </c>
-      <c r="C7" s="8">
-        <v>6</v>
-      </c>
-      <c r="D7" s="8">
-        <v>9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>6</v>
-      </c>
-      <c r="F7" s="8">
-        <v>5</v>
-      </c>
-      <c r="G7" s="8">
-        <v>8</v>
-      </c>
-      <c r="H7" s="8">
-        <v>8</v>
-      </c>
-      <c r="I7" s="8">
-        <v>8</v>
-      </c>
-      <c r="J7" s="8">
-        <v>11</v>
-      </c>
-      <c r="K7" s="8">
-        <v>13</v>
-      </c>
-      <c r="L7" s="8">
-        <v>14</v>
-      </c>
-      <c r="M7" s="8">
-        <v>16</v>
-      </c>
-      <c r="N7" s="8">
-        <v>19</v>
-      </c>
-      <c r="O7" s="8">
-        <v>23</v>
-      </c>
-      <c r="P7" s="8">
-        <v>45</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>45</v>
-      </c>
-      <c r="R7" s="8">
-        <v>45</v>
-      </c>
-      <c r="S7" s="8">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8">
-        <v>19</v>
-      </c>
-      <c r="C8" s="8">
-        <v>19</v>
-      </c>
-      <c r="D8" s="8">
-        <v>16</v>
-      </c>
-      <c r="E8" s="8">
-        <v>16</v>
-      </c>
-      <c r="F8" s="8">
-        <v>16</v>
-      </c>
-      <c r="G8" s="8">
-        <v>19</v>
-      </c>
-      <c r="H8" s="8">
-        <v>16</v>
-      </c>
-      <c r="I8" s="8">
-        <v>14</v>
-      </c>
-      <c r="J8" s="8">
-        <v>13</v>
-      </c>
-      <c r="K8" s="8">
-        <v>15</v>
-      </c>
-      <c r="L8" s="8">
-        <v>17</v>
-      </c>
-      <c r="M8" s="8">
-        <v>17</v>
-      </c>
-      <c r="N8" s="8">
-        <v>20</v>
-      </c>
-      <c r="O8" s="8">
-        <v>45</v>
-      </c>
-      <c r="P8" s="8">
-        <v>45</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>45</v>
-      </c>
-      <c r="R8" s="8">
-        <v>45</v>
-      </c>
-      <c r="S8" s="8">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>3</v>
-      </c>
-      <c r="B9" s="8">
-        <v>19</v>
-      </c>
-      <c r="C9" s="8">
-        <v>19</v>
-      </c>
-      <c r="D9" s="8">
-        <v>16</v>
-      </c>
-      <c r="E9" s="8">
-        <v>16</v>
-      </c>
-      <c r="F9" s="8">
-        <v>16</v>
-      </c>
-      <c r="G9" s="8">
-        <v>19</v>
-      </c>
-      <c r="H9" s="8">
-        <v>16</v>
-      </c>
-      <c r="I9" s="8">
-        <v>14</v>
-      </c>
-      <c r="J9" s="8">
-        <v>15</v>
-      </c>
-      <c r="K9" s="8">
-        <v>18</v>
-      </c>
-      <c r="L9" s="8">
-        <v>19</v>
-      </c>
-      <c r="M9" s="8">
-        <v>19</v>
-      </c>
-      <c r="N9" s="8">
-        <v>20</v>
-      </c>
-      <c r="O9" s="8">
-        <v>45</v>
-      </c>
-      <c r="P9" s="8">
-        <v>45</v>
-      </c>
-      <c r="Q9" s="8">
-        <v>45</v>
-      </c>
-      <c r="R9" s="8">
-        <v>45</v>
-      </c>
-      <c r="S9" s="8">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>3</v>
-      </c>
-      <c r="B10" s="8">
-        <v>19</v>
-      </c>
-      <c r="C10" s="8">
-        <v>19</v>
-      </c>
-      <c r="D10" s="8">
-        <v>16</v>
-      </c>
-      <c r="E10" s="8">
-        <v>16</v>
-      </c>
-      <c r="F10" s="8">
-        <v>16</v>
-      </c>
-      <c r="G10" s="8">
-        <v>19</v>
-      </c>
-      <c r="H10" s="8">
-        <v>17</v>
-      </c>
-      <c r="I10" s="8">
-        <v>16</v>
-      </c>
-      <c r="J10" s="8">
-        <v>17</v>
-      </c>
-      <c r="K10" s="8">
-        <v>20</v>
-      </c>
-      <c r="L10" s="8">
-        <v>20</v>
-      </c>
-      <c r="M10" s="8">
-        <v>20</v>
-      </c>
-      <c r="N10" s="8">
-        <v>21</v>
-      </c>
-      <c r="O10" s="8">
-        <v>45</v>
-      </c>
-      <c r="P10" s="8">
-        <v>45</v>
-      </c>
-      <c r="Q10" s="8">
-        <v>45</v>
-      </c>
-      <c r="R10" s="8">
-        <v>48</v>
-      </c>
-      <c r="S10" s="8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>3</v>
-      </c>
-      <c r="B11" s="8">
-        <v>19</v>
-      </c>
-      <c r="C11" s="8">
-        <v>19</v>
-      </c>
-      <c r="D11" s="8">
-        <v>18</v>
-      </c>
-      <c r="E11" s="8">
-        <v>17</v>
-      </c>
-      <c r="F11" s="8">
-        <v>16</v>
-      </c>
-      <c r="G11" s="8">
-        <v>19</v>
-      </c>
-      <c r="H11" s="8">
-        <v>18</v>
-      </c>
-      <c r="I11" s="8">
-        <v>19</v>
-      </c>
-      <c r="J11" s="8">
-        <v>20</v>
-      </c>
-      <c r="K11" s="8">
-        <v>20</v>
-      </c>
-      <c r="L11" s="8">
-        <v>21</v>
-      </c>
-      <c r="M11" s="8">
-        <v>21</v>
-      </c>
-      <c r="N11" s="8">
-        <v>21</v>
-      </c>
-      <c r="O11" s="8">
-        <v>45</v>
-      </c>
-      <c r="P11" s="8">
-        <v>45</v>
-      </c>
-      <c r="Q11" s="8">
-        <v>47</v>
-      </c>
-      <c r="R11" s="8">
-        <v>49</v>
-      </c>
-      <c r="S11" s="8">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>3</v>
-      </c>
-      <c r="B12" s="8">
-        <v>21</v>
-      </c>
-      <c r="C12" s="8">
-        <v>21</v>
-      </c>
-      <c r="D12" s="8">
-        <v>21</v>
-      </c>
-      <c r="E12" s="8">
-        <v>20</v>
-      </c>
-      <c r="F12" s="8">
-        <v>19</v>
-      </c>
-      <c r="G12" s="8">
-        <v>20</v>
-      </c>
-      <c r="H12" s="8">
-        <v>21</v>
-      </c>
-      <c r="I12" s="8">
-        <v>22</v>
-      </c>
-      <c r="J12" s="8">
-        <v>22</v>
-      </c>
-      <c r="K12" s="8">
-        <v>22</v>
-      </c>
-      <c r="L12" s="8">
-        <v>22</v>
-      </c>
-      <c r="M12" s="8">
-        <v>22</v>
-      </c>
-      <c r="N12" s="8">
-        <v>22</v>
-      </c>
-      <c r="O12" s="8">
-        <v>46</v>
-      </c>
-      <c r="P12" s="8">
-        <v>47</v>
-      </c>
-      <c r="Q12" s="8">
-        <v>50</v>
-      </c>
-      <c r="R12" s="8">
-        <v>53</v>
-      </c>
-      <c r="S12" s="8">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>3</v>
-      </c>
-      <c r="B13" s="8">
-        <v>21</v>
-      </c>
-      <c r="C13" s="8">
-        <v>21</v>
-      </c>
-      <c r="D13" s="8">
-        <v>22</v>
-      </c>
-      <c r="E13" s="8">
-        <v>22</v>
-      </c>
-      <c r="F13" s="8">
-        <v>22</v>
-      </c>
-      <c r="G13" s="8">
-        <v>22</v>
-      </c>
-      <c r="H13" s="8">
-        <v>22</v>
-      </c>
-      <c r="I13" s="8">
-        <v>26</v>
-      </c>
-      <c r="J13" s="8">
-        <v>26</v>
-      </c>
-      <c r="K13" s="8">
-        <v>26</v>
-      </c>
-      <c r="L13" s="8">
-        <v>26</v>
-      </c>
-      <c r="M13" s="8">
-        <v>26</v>
-      </c>
-      <c r="N13" s="8">
-        <v>46</v>
-      </c>
-      <c r="O13" s="8">
-        <v>46</v>
-      </c>
-      <c r="P13" s="8">
-        <v>47</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>52</v>
-      </c>
-      <c r="R13" s="8">
-        <v>56</v>
-      </c>
-      <c r="S13" s="8">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>3</v>
-      </c>
-      <c r="B14" s="8">
-        <v>21</v>
-      </c>
-      <c r="C14" s="8">
-        <v>21</v>
-      </c>
-      <c r="D14" s="8">
-        <v>22</v>
-      </c>
-      <c r="E14" s="8">
-        <v>22</v>
-      </c>
-      <c r="F14" s="8">
-        <v>22</v>
-      </c>
-      <c r="G14" s="8">
-        <v>22</v>
-      </c>
-      <c r="H14" s="8">
-        <v>22</v>
-      </c>
-      <c r="I14" s="8">
-        <v>27</v>
-      </c>
-      <c r="J14" s="8">
-        <v>27</v>
-      </c>
-      <c r="K14" s="8">
-        <v>27</v>
-      </c>
-      <c r="L14" s="8">
-        <v>27</v>
-      </c>
-      <c r="M14" s="8">
-        <v>27</v>
-      </c>
-      <c r="N14" s="8">
-        <v>46</v>
-      </c>
-      <c r="O14" s="8">
-        <v>46</v>
-      </c>
-      <c r="P14" s="8">
-        <v>50</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>54</v>
-      </c>
-      <c r="R14" s="8">
-        <v>58</v>
-      </c>
-      <c r="S14" s="8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>3</v>
-      </c>
-      <c r="B15" s="8">
-        <v>21</v>
-      </c>
-      <c r="C15" s="8">
-        <v>21</v>
-      </c>
-      <c r="D15" s="8">
-        <v>22</v>
-      </c>
-      <c r="E15" s="8">
-        <v>23</v>
-      </c>
-      <c r="F15" s="8">
-        <v>23</v>
-      </c>
-      <c r="G15" s="8">
-        <v>22</v>
-      </c>
-      <c r="H15" s="8">
-        <v>22</v>
-      </c>
-      <c r="I15" s="8">
-        <v>27</v>
-      </c>
-      <c r="J15" s="8">
-        <v>27</v>
-      </c>
-      <c r="K15" s="8">
-        <v>28</v>
-      </c>
-      <c r="L15" s="8">
-        <v>27</v>
-      </c>
-      <c r="M15" s="8">
-        <v>46</v>
-      </c>
-      <c r="N15" s="8">
-        <v>46</v>
-      </c>
-      <c r="O15" s="8">
-        <v>48</v>
-      </c>
-      <c r="P15" s="8">
-        <v>54</v>
-      </c>
-      <c r="Q15" s="8">
-        <v>57</v>
-      </c>
-      <c r="R15" s="8">
-        <v>60</v>
-      </c>
-      <c r="S15" s="8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>3</v>
-      </c>
-      <c r="B16" s="8">
-        <v>21</v>
-      </c>
-      <c r="C16" s="8">
-        <v>21</v>
-      </c>
-      <c r="D16" s="8">
-        <v>22</v>
-      </c>
-      <c r="E16" s="8">
-        <v>23</v>
-      </c>
-      <c r="F16" s="8">
-        <v>23</v>
-      </c>
-      <c r="G16" s="8">
-        <v>23</v>
-      </c>
-      <c r="H16" s="8">
-        <v>23</v>
-      </c>
-      <c r="I16" s="8">
-        <v>27</v>
-      </c>
-      <c r="J16" s="8">
-        <v>28</v>
-      </c>
-      <c r="K16" s="8">
-        <v>28</v>
-      </c>
-      <c r="L16" s="8">
-        <v>46</v>
-      </c>
-      <c r="M16" s="8">
-        <v>46</v>
-      </c>
-      <c r="N16" s="8">
-        <v>46</v>
-      </c>
-      <c r="O16" s="8">
-        <v>49</v>
-      </c>
-      <c r="P16" s="8">
-        <v>55</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>57</v>
-      </c>
-      <c r="R16" s="8">
-        <v>60</v>
-      </c>
-      <c r="S16" s="8">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>3</v>
-      </c>
-      <c r="B17" s="8">
-        <v>21</v>
-      </c>
-      <c r="C17" s="8">
-        <v>21</v>
-      </c>
-      <c r="D17" s="8">
-        <v>22</v>
-      </c>
-      <c r="E17" s="8">
-        <v>23</v>
-      </c>
-      <c r="F17" s="8">
-        <v>23</v>
-      </c>
-      <c r="G17" s="8">
-        <v>23</v>
-      </c>
-      <c r="H17" s="8">
-        <v>23</v>
-      </c>
-      <c r="I17" s="8">
-        <v>27</v>
-      </c>
-      <c r="J17" s="8">
-        <v>28</v>
-      </c>
-      <c r="K17" s="8">
-        <v>28</v>
-      </c>
-      <c r="L17" s="8">
-        <v>46</v>
-      </c>
-      <c r="M17" s="8">
-        <v>46</v>
-      </c>
-      <c r="N17" s="8">
-        <v>46</v>
-      </c>
-      <c r="O17" s="8">
-        <v>60</v>
-      </c>
-      <c r="P17" s="8">
-        <v>60</v>
-      </c>
-      <c r="Q17" s="8">
-        <v>60</v>
-      </c>
-      <c r="R17" s="8">
-        <v>60</v>
-      </c>
-      <c r="S17" s="8">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
test Stage 1 1.8 map
</commit_message>
<xml_diff>
--- a/E85Blend calculator.xlsx
+++ b/E85Blend calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOW\RX8-E85-Vtune\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783D7ED5-4113-4F35-9478-71FEE089C430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69423CD1-A2CE-46CF-ACD4-F7012ED54CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
+    <workbookView xWindow="2070" yWindow="6030" windowWidth="21600" windowHeight="9450" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
   </bookViews>
   <sheets>
     <sheet name="Blend" sheetId="1" r:id="rId1"/>
@@ -939,7 +939,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,6 +949,7 @@
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1004,7 +1005,7 @@
         <v>6.8128151778621665E-2</v>
       </c>
       <c r="J2" s="19">
-        <f>B$14/H2</f>
+        <f t="shared" ref="J2:J22" si="0">B$14/H2</f>
         <v>0.94358607515080162</v>
       </c>
     </row>
@@ -1030,11 +1031,11 @@
         <v>14.39321</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I22" si="0">1/H3</f>
+        <f t="shared" ref="I3:I22" si="1">1/H3</f>
         <v>6.9477204876466053E-2</v>
       </c>
       <c r="J3" s="19">
-        <f>B$14/H3</f>
+        <f t="shared" si="0"/>
         <v>0.96227068180065456</v>
       </c>
     </row>
@@ -1047,36 +1048,36 @@
       </c>
       <c r="C4" s="3"/>
       <c r="G4" s="20">
-        <f t="shared" ref="G4:G14" si="1">G3+5%</f>
+        <f t="shared" ref="G4:G14" si="2">G3+5%</f>
         <v>0.1</v>
       </c>
       <c r="H4">
         <v>14.1082</v>
       </c>
       <c r="I4">
+        <f t="shared" si="1"/>
+        <v>7.0880764378163055E-2</v>
+      </c>
+      <c r="J4" s="19">
         <f t="shared" si="0"/>
-        <v>7.0880764378163055E-2</v>
-      </c>
-      <c r="J4" s="19">
-        <f>B$14/H4</f>
         <v>0.98171021108291623</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="G5" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="H5">
         <v>13.82319</v>
       </c>
       <c r="I5">
+        <f t="shared" si="1"/>
+        <v>7.2342201763847563E-2</v>
+      </c>
+      <c r="J5" s="19">
         <f t="shared" si="0"/>
-        <v>7.2342201763847563E-2</v>
-      </c>
-      <c r="J5" s="19">
-        <f>B$14/H5</f>
         <v>1.0019513585503779</v>
       </c>
     </row>
@@ -1089,18 +1090,18 @@
       </c>
       <c r="C6" s="3"/>
       <c r="G6" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
       <c r="H6">
         <v>13.538180000000001</v>
       </c>
       <c r="I6">
+        <f t="shared" si="1"/>
+        <v>7.3865172423471986E-2</v>
+      </c>
+      <c r="J6" s="19">
         <f t="shared" si="0"/>
-        <v>7.3865172423471986E-2</v>
-      </c>
-      <c r="J6" s="19">
-        <f>B$14/H6</f>
         <v>1.0230447519533643</v>
       </c>
     </row>
@@ -1114,18 +1115,18 @@
         <v>60</v>
       </c>
       <c r="G7" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="H7">
         <v>13.253170000000001</v>
       </c>
       <c r="I7">
+        <f t="shared" si="1"/>
+        <v>7.5453646184271375E-2</v>
+      </c>
+      <c r="J7" s="19">
         <f t="shared" si="0"/>
-        <v>7.5453646184271375E-2</v>
-      </c>
-      <c r="J7" s="19">
-        <f>B$14/H7</f>
         <v>1.0450453740501329</v>
       </c>
     </row>
@@ -1139,18 +1140,18 @@
         <v>0</v>
       </c>
       <c r="G8" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="H8">
         <v>12.968159999999999</v>
       </c>
       <c r="I8">
+        <f t="shared" si="1"/>
+        <v>7.7111941863764799E-2</v>
+      </c>
+      <c r="J8" s="19">
         <f t="shared" si="0"/>
-        <v>7.7111941863764799E-2</v>
-      </c>
-      <c r="J8" s="19">
-        <f>B$14/H8</f>
         <v>1.068013041171608</v>
       </c>
     </row>
@@ -1172,18 +1173,18 @@
         <v>8.15625</v>
       </c>
       <c r="G9" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.35</v>
       </c>
       <c r="H9">
         <v>12.683149999999999</v>
       </c>
       <c r="I9">
+        <f t="shared" si="1"/>
+        <v>7.8844766481512882E-2</v>
+      </c>
+      <c r="J9" s="19">
         <f t="shared" si="0"/>
-        <v>7.8844766481512882E-2</v>
-      </c>
-      <c r="J9" s="19">
-        <f>B$14/H9</f>
         <v>1.0920129463106563</v>
       </c>
     </row>
@@ -1205,18 +1206,18 @@
         <v>0.73979591836734704</v>
       </c>
       <c r="G10" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="H10">
         <v>12.39812</v>
       </c>
       <c r="I10">
+        <f t="shared" si="1"/>
+        <v>8.0657389991385789E-2</v>
+      </c>
+      <c r="J10" s="19">
         <f t="shared" si="0"/>
-        <v>8.0657389991385789E-2</v>
-      </c>
-      <c r="J10" s="19">
-        <f>B$14/H10</f>
         <v>1.1171180791926516</v>
       </c>
     </row>
@@ -1238,35 +1239,35 @@
         <v>1.260204081632653</v>
       </c>
       <c r="G11" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="H11">
         <v>12.11313</v>
       </c>
       <c r="I11">
+        <f t="shared" si="1"/>
+        <v>8.2555045640556976E-2</v>
+      </c>
+      <c r="J11" s="19">
         <f t="shared" si="0"/>
-        <v>8.2555045640556976E-2</v>
-      </c>
-      <c r="J11" s="19">
-        <f>B$14/H11</f>
         <v>1.1434009211491991</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G12" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.49999999999999994</v>
       </c>
       <c r="H12">
         <v>11.82812</v>
       </c>
       <c r="I12">
+        <f t="shared" si="1"/>
+        <v>8.4544289371430117E-2</v>
+      </c>
+      <c r="J12" s="19">
         <f t="shared" si="0"/>
-        <v>8.4544289371430117E-2</v>
-      </c>
-      <c r="J12" s="19">
-        <f>B$14/H12</f>
         <v>1.1709522730577639</v>
       </c>
     </row>
@@ -1284,18 +1285,18 @@
         <v>29</v>
       </c>
       <c r="G13" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.54999999999999993</v>
       </c>
       <c r="H13">
         <v>11.54311</v>
       </c>
       <c r="I13">
+        <f t="shared" si="1"/>
+        <v>8.6631765616025494E-2</v>
+      </c>
+      <c r="J13" s="19">
         <f t="shared" si="0"/>
-        <v>8.6631765616025494E-2</v>
-      </c>
-      <c r="J13" s="19">
-        <f>B$14/H13</f>
         <v>1.199864161391514</v>
       </c>
     </row>
@@ -1311,18 +1312,18 @@
         <v>7.2201311118048853E-2</v>
       </c>
       <c r="G14" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="H14">
         <v>11.258100000000001</v>
       </c>
       <c r="I14">
+        <f t="shared" si="1"/>
+        <v>8.882493493573515E-2</v>
+      </c>
+      <c r="J14" s="19">
         <f t="shared" si="0"/>
-        <v>8.882493493573515E-2</v>
-      </c>
-      <c r="J14" s="19">
-        <f>B$14/H14</f>
         <v>1.2302399161492612</v>
       </c>
     </row>
@@ -1337,132 +1338,132 @@
         <v>10.973089999999999</v>
       </c>
       <c r="I15">
+        <f t="shared" si="1"/>
+        <v>9.1132033000731791E-2</v>
+      </c>
+      <c r="J15" s="19">
         <f t="shared" si="0"/>
-        <v>9.1132033000731791E-2</v>
-      </c>
-      <c r="J15" s="19">
-        <f>B$14/H15</f>
         <v>1.2621936027135474</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="G16" s="20">
-        <f t="shared" ref="G16:G22" si="2">G15+5%</f>
+        <f t="shared" ref="G16:G22" si="3">G15+5%</f>
         <v>0.70000000000000007</v>
       </c>
       <c r="H16">
         <v>10.688079999999999</v>
       </c>
       <c r="I16">
+        <f t="shared" si="1"/>
+        <v>9.3562173935823834E-2</v>
+      </c>
+      <c r="J16" s="19">
         <f t="shared" si="0"/>
-        <v>9.3562173935823834E-2</v>
-      </c>
-      <c r="J16" s="19">
-        <f>B$14/H16</f>
         <v>1.2958514532076857</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="G17" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.75000000000000011</v>
       </c>
       <c r="H17">
         <v>10.40307</v>
       </c>
       <c r="I17">
+        <f t="shared" si="1"/>
+        <v>9.6125470654335701E-2</v>
+      </c>
+      <c r="J17" s="19">
         <f t="shared" si="0"/>
-        <v>9.6125470654335701E-2</v>
-      </c>
-      <c r="J17" s="19">
-        <f>B$14/H17</f>
         <v>1.3313535331397366</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G18" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.80000000000000016</v>
       </c>
       <c r="H18">
         <v>10.11806</v>
       </c>
       <c r="I18">
+        <f t="shared" si="1"/>
+        <v>9.8833175529696407E-2</v>
+      </c>
+      <c r="J18" s="19">
         <f t="shared" si="0"/>
-        <v>9.8833175529696407E-2</v>
-      </c>
-      <c r="J18" s="19">
-        <f>B$14/H18</f>
         <v>1.368855689727082</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G19" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.8500000000000002</v>
       </c>
       <c r="H19">
         <v>9.8330500000000001</v>
       </c>
       <c r="I19">
+        <f t="shared" si="1"/>
+        <v>0.10169784553114242</v>
+      </c>
+      <c r="J19" s="19">
         <f t="shared" si="0"/>
-        <v>0.10169784553114242</v>
-      </c>
-      <c r="J19" s="19">
-        <f>B$14/H19</f>
         <v>1.4085318390529895</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G20" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.90000000000000024</v>
       </c>
       <c r="H20">
         <v>9.5480400000000003</v>
       </c>
       <c r="I20">
+        <f t="shared" si="1"/>
+        <v>0.10473353693532914</v>
+      </c>
+      <c r="J20" s="19">
         <f t="shared" si="0"/>
-        <v>0.10473353693532914</v>
-      </c>
-      <c r="J20" s="19">
-        <f>B$14/H20</f>
         <v>1.4505766628543659</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G21" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.95000000000000029</v>
       </c>
       <c r="H21">
         <v>9.2630300000000005</v>
       </c>
       <c r="I21">
+        <f t="shared" si="1"/>
+        <v>0.10795603598390591</v>
+      </c>
+      <c r="J21" s="19">
         <f t="shared" si="0"/>
-        <v>0.10795603598390591</v>
-      </c>
-      <c r="J21" s="19">
-        <f>B$14/H21</f>
         <v>1.4952088031669981</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G22" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="H22">
         <v>8.9880200000000006</v>
       </c>
       <c r="I22">
+        <f t="shared" si="1"/>
+        <v>0.11125920948106478</v>
+      </c>
+      <c r="J22" s="19">
         <f t="shared" si="0"/>
-        <v>0.11125920948106478</v>
-      </c>
-      <c r="J22" s="19">
-        <f>B$14/H22</f>
         <v>1.5409582978231022</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add V1.10 E85 VE + DWELL AEM coils
</commit_message>
<xml_diff>
--- a/E85Blend calculator.xlsx
+++ b/E85Blend calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOW\RX8-E85-Vtune\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69423CD1-A2CE-46CF-ACD4-F7012ED54CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477478CD-1CE3-434D-AF58-DC3EA4558AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="6030" windowWidth="21600" windowHeight="9450" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
   </bookViews>
   <sheets>
     <sheet name="Blend" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Gasoline</t>
   </si>
@@ -143,6 +143,21 @@
   </si>
   <si>
     <t>Delta VS Default RX8 Stoich</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>DutyCycle</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>AEM</t>
+  </si>
+  <si>
+    <t>Addition</t>
   </si>
 </sst>
 </file>
@@ -293,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -319,6 +334,15 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C507529D-A20D-4ABB-AAE4-BE6AA5385A82}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12562,10 +12586,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC026DA-F509-4385-B6B3-72E60872EBDC}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12950,6 +12974,211 @@
         <v>3.1440000000000001</v>
       </c>
     </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="23">
+        <v>-30</v>
+      </c>
+      <c r="C15" s="23">
+        <v>-20</v>
+      </c>
+      <c r="D15" s="23">
+        <v>-10</v>
+      </c>
+      <c r="E15" s="23">
+        <v>0</v>
+      </c>
+      <c r="F15" s="23">
+        <v>10</v>
+      </c>
+      <c r="G15" s="23">
+        <v>20</v>
+      </c>
+      <c r="H15" s="23">
+        <v>30</v>
+      </c>
+      <c r="I15" s="23">
+        <v>40</v>
+      </c>
+      <c r="J15" s="23">
+        <v>50</v>
+      </c>
+      <c r="K15" s="23">
+        <v>60</v>
+      </c>
+      <c r="L15" s="23">
+        <v>70</v>
+      </c>
+      <c r="M15" s="23">
+        <v>80</v>
+      </c>
+      <c r="N15" s="23">
+        <v>90</v>
+      </c>
+      <c r="O15" s="23">
+        <v>100</v>
+      </c>
+      <c r="P15" s="23">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="22">
+        <v>101.8</v>
+      </c>
+      <c r="C16" s="22">
+        <v>60.84</v>
+      </c>
+      <c r="D16" s="22">
+        <v>35</v>
+      </c>
+      <c r="E16" s="22">
+        <v>35</v>
+      </c>
+      <c r="F16" s="22">
+        <v>35</v>
+      </c>
+      <c r="G16" s="22">
+        <v>35</v>
+      </c>
+      <c r="H16" s="22">
+        <v>35</v>
+      </c>
+      <c r="I16" s="22">
+        <v>35</v>
+      </c>
+      <c r="J16" s="22">
+        <v>35</v>
+      </c>
+      <c r="K16" s="22">
+        <v>9</v>
+      </c>
+      <c r="L16" s="22">
+        <v>8</v>
+      </c>
+      <c r="M16" s="22">
+        <v>5.2480000000000002</v>
+      </c>
+      <c r="N16" s="22">
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="O16" s="22">
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="P16" s="22">
+        <v>3.1440000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="24">
+        <v>0.4</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="F17" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0</v>
+      </c>
+      <c r="I17" s="24">
+        <v>0</v>
+      </c>
+      <c r="J17" s="24">
+        <v>0</v>
+      </c>
+      <c r="K17" s="24">
+        <v>0</v>
+      </c>
+      <c r="L17" s="24">
+        <v>0</v>
+      </c>
+      <c r="M17" s="24">
+        <v>0</v>
+      </c>
+      <c r="N17" s="24">
+        <v>0</v>
+      </c>
+      <c r="O17" s="24">
+        <v>0</v>
+      </c>
+      <c r="P17" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="25">
+        <v>152.69999999999999</v>
+      </c>
+      <c r="C18" s="25">
+        <v>91.26</v>
+      </c>
+      <c r="D18" s="25">
+        <v>49</v>
+      </c>
+      <c r="E18" s="25">
+        <v>45.5</v>
+      </c>
+      <c r="F18" s="25">
+        <v>42</v>
+      </c>
+      <c r="G18" s="25">
+        <v>38.5</v>
+      </c>
+      <c r="H18" s="25">
+        <v>35</v>
+      </c>
+      <c r="I18" s="25">
+        <v>35</v>
+      </c>
+      <c r="J18" s="25">
+        <v>35</v>
+      </c>
+      <c r="K18" s="25">
+        <v>9</v>
+      </c>
+      <c r="L18" s="25">
+        <v>8</v>
+      </c>
+      <c r="M18" s="25">
+        <v>5.2480000000000002</v>
+      </c>
+      <c r="N18" s="25">
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="O18" s="25">
+        <v>3.1440000000000001</v>
+      </c>
+      <c r="P18" s="25">
+        <v>3.1440000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12957,15 +13186,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745AD7B9-4B1D-4E8C-A42C-E86EAA5F24F9}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>7.4020000000000001</v>
       </c>
@@ -12994,7 +13223,7 @@
         <v>1.5429999999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>6.5940000000000003</v>
       </c>
@@ -13023,7 +13252,7 @@
         <v>1.5429999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>5.9379999999999997</v>
       </c>
@@ -13052,7 +13281,7 @@
         <v>1.5429999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>5.4489999999999998</v>
       </c>
@@ -13081,7 +13310,7 @@
         <v>1.5429999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>5.0469999999999997</v>
       </c>
@@ -13110,7 +13339,7 @@
         <v>1.5429999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4.7190000000000003</v>
       </c>
@@ -13139,7 +13368,7 @@
         <v>1.5429999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4.3159999999999998</v>
       </c>
@@ -13168,7 +13397,7 @@
         <v>1.5429999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3.6640000000000001</v>
       </c>
@@ -13197,7 +13426,7 @@
         <v>1.5429999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>3.1720000000000002</v>
       </c>
@@ -13224,6 +13453,736 @@
       </c>
       <c r="I9" s="2">
         <v>1.5429999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B11">
+        <f>A11+1000</f>
+        <v>2000</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:H11" si="0">B11+1000</f>
+        <v>3000</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>7000</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="I11">
+        <f>H11+1000</f>
+        <v>9000</v>
+      </c>
+      <c r="J11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>(60/A11*1000)</f>
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:H12" si="1">(60/B11*1000)</f>
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>8.5714285714285712</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="I12">
+        <f>(60/I11*1000)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="J12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" ref="A13:H13" si="2">A12*40%</f>
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>3.4285714285714288</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <f>I12*40%</f>
+        <v>2.666666666666667</v>
+      </c>
+      <c r="J13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>7.4</v>
+      </c>
+      <c r="B16">
+        <v>5.9</v>
+      </c>
+      <c r="C16">
+        <v>5.5</v>
+      </c>
+      <c r="D16">
+        <v>5.5</v>
+      </c>
+      <c r="E16">
+        <v>4.8</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>3.4</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6.6</v>
+      </c>
+      <c r="B17">
+        <v>5.2</v>
+      </c>
+      <c r="C17">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D17">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E17">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>3.4</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5.9</v>
+      </c>
+      <c r="B18">
+        <v>4.7</v>
+      </c>
+      <c r="C18">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>3.4</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5.4</v>
+      </c>
+      <c r="B19">
+        <v>4.3</v>
+      </c>
+      <c r="C19">
+        <v>3.8</v>
+      </c>
+      <c r="D19">
+        <v>3.5</v>
+      </c>
+      <c r="E19">
+        <v>3.5</v>
+      </c>
+      <c r="F19">
+        <v>3.5</v>
+      </c>
+      <c r="G19">
+        <v>3.4</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>3.5</v>
+      </c>
+      <c r="D20">
+        <v>3.2</v>
+      </c>
+      <c r="E20">
+        <v>3.1</v>
+      </c>
+      <c r="F20">
+        <v>3.1</v>
+      </c>
+      <c r="G20">
+        <v>3.1</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4.7</v>
+      </c>
+      <c r="B21">
+        <v>3.7</v>
+      </c>
+      <c r="C21">
+        <v>3.3</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>2.8</v>
+      </c>
+      <c r="F21">
+        <v>2.8</v>
+      </c>
+      <c r="G21">
+        <v>2.8</v>
+      </c>
+      <c r="H21">
+        <v>2.8</v>
+      </c>
+      <c r="I21">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4.3</v>
+      </c>
+      <c r="B22">
+        <v>3.7</v>
+      </c>
+      <c r="C22">
+        <v>3.1</v>
+      </c>
+      <c r="D22">
+        <v>2.8</v>
+      </c>
+      <c r="E22">
+        <v>2.6</v>
+      </c>
+      <c r="F22">
+        <v>2.6</v>
+      </c>
+      <c r="G22">
+        <v>2.6</v>
+      </c>
+      <c r="H22">
+        <v>2.6</v>
+      </c>
+      <c r="I22">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3.7</v>
+      </c>
+      <c r="B23">
+        <v>3.3</v>
+      </c>
+      <c r="C23">
+        <v>2.9</v>
+      </c>
+      <c r="D23">
+        <v>2.6</v>
+      </c>
+      <c r="E23">
+        <v>2.4</v>
+      </c>
+      <c r="F23">
+        <v>2.4</v>
+      </c>
+      <c r="G23">
+        <v>2.4</v>
+      </c>
+      <c r="H23">
+        <v>2.4</v>
+      </c>
+      <c r="I23">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3.2</v>
+      </c>
+      <c r="B24">
+        <v>3.1</v>
+      </c>
+      <c r="C24">
+        <v>2.7</v>
+      </c>
+      <c r="D24">
+        <v>2.5</v>
+      </c>
+      <c r="E24">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I24">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f>A16*100/A$12</f>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ref="B27:I27" si="3">B16*100/B$12</f>
+        <v>19.666666666666668</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="3"/>
+        <v>27.5</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="3"/>
+        <v>36.666666666666664</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>39.666666666666664</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" ref="A28:I28" si="4">A17*100/A$12</f>
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="4"/>
+        <v>17.333333333333332</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="4"/>
+        <v>22.999999999999996</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="4"/>
+        <v>30.666666666666664</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>38.333333333333329</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>39.666666666666664</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" ref="A29:I29" si="5">A18*100/A$12</f>
+        <v>9.8333333333333339</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="5"/>
+        <v>15.666666666666666</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="5"/>
+        <v>20.499999999999996</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="5"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="5"/>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>39.666666666666664</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="5"/>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" ref="A30:I30" si="6">A19*100/A$12</f>
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="6"/>
+        <v>14.333333333333334</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="6"/>
+        <v>23.333333333333332</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="6"/>
+        <v>29.166666666666668</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="6"/>
+        <v>35</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="6"/>
+        <v>39.666666666666664</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="6"/>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" ref="A31:I31" si="7">A20*100/A$12</f>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="7"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="7"/>
+        <v>17.5</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="7"/>
+        <v>21.333333333333332</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="7"/>
+        <v>25.833333333333332</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="7"/>
+        <v>31</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="7"/>
+        <v>36.166666666666664</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="7"/>
+        <v>40</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="7"/>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" ref="A32:I32" si="8">A21*100/A$12</f>
+        <v>7.833333333333333</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="8"/>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="8"/>
+        <v>16.5</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="8"/>
+        <v>23.333333333333332</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="8"/>
+        <v>32.666666666666664</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="8"/>
+        <v>37.333333333333336</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="8"/>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" ref="A33:I33" si="9">A22*100/A$12</f>
+        <v>7.166666666666667</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="9"/>
+        <v>12.333333333333334</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="9"/>
+        <v>15.5</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="9"/>
+        <v>18.666666666666668</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="9"/>
+        <v>21.666666666666668</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="9"/>
+        <v>30.333333333333336</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="9"/>
+        <v>34.666666666666664</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="9"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" ref="A34:I34" si="10">A23*100/A$12</f>
+        <v>6.166666666666667</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="10"/>
+        <v>14.5</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="10"/>
+        <v>17.333333333333332</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="10"/>
+        <v>20</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="10"/>
+        <v>24</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="10"/>
+        <v>28</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="10"/>
+        <v>32</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="10"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" ref="A35:I35" si="11">A24*100/A$12</f>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="11"/>
+        <v>10.333333333333334</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="11"/>
+        <v>13.5</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="11"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="11"/>
+        <v>19.166666666666664</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="11"/>
+        <v>22.000000000000004</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="11"/>
+        <v>25.666666666666671</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="11"/>
+        <v>29.333333333333336</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="11"/>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -13236,7 +14195,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Volumetry Efficiency Table tune back
</commit_message>
<xml_diff>
--- a/E85Blend calculator.xlsx
+++ b/E85Blend calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOW\RX8-E85-Vtune\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D68665C-E754-477E-862A-C6C33186B3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474E7037-1BC4-46D6-B980-777F09E04016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="1740" windowWidth="21600" windowHeight="11295" firstSheet="5" activeTab="7" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{90F246BF-DB6B-4892-AB09-839B6BF21924}"/>
   </bookViews>
   <sheets>
     <sheet name="Blend" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="AFR 1 (RX8 Evolve 2006 UK)" sheetId="7" r:id="rId13"/>
     <sheet name="AFR 2 (RX8 Evolve 2006 UK)" sheetId="8" r:id="rId14"/>
     <sheet name="AFR 3 (RX8 Evolve 2006 UK)" sheetId="9" r:id="rId15"/>
+    <sheet name="test" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Gasoline</t>
   </si>
@@ -223,15 +224,26 @@
   <si>
     <t>30% More</t>
   </si>
+  <si>
+    <t>RRP Table</t>
+  </si>
+  <si>
+    <t>Delta vs Stock</t>
+  </si>
+  <si>
+    <t>13.85 = 0.07196</t>
+  </si>
+  <si>
+    <t>9.83 = 0.090564117</t>
+  </si>
+  <si>
+    <t>8.8 = 0.094951175</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#&quot; &quot;?/10"/>
-    <numFmt numFmtId="165" formatCode="#&quot; &quot;??/100"/>
-  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -408,8 +420,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1029,7 +1039,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C507529D-A20D-4ABB-AAE4-BE6AA5385A82}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
@@ -1047,7 +1057,7 @@
     <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1076,8 +1086,9 @@
       <c r="K1" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1109,8 +1120,12 @@
         <f>H2*$J$2</f>
         <v>13.850163999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>-0.004574 * K2 + 0.135345</f>
+        <v>7.1994349863999996E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1143,8 +1158,15 @@
         <f t="shared" ref="K3:K22" si="2">H3*$J$2</f>
         <v>13.58123253272127</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f t="shared" ref="L3:L22" si="3">-0.004574 * K3 + 0.135345</f>
+        <v>7.3224442395332906E-2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1153,7 +1175,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="G4" s="20">
-        <f t="shared" ref="G4:G14" si="3">G3+5%</f>
+        <f t="shared" ref="G4:G14" si="4">G3+5%</f>
         <v>0.1</v>
       </c>
       <c r="H4">
@@ -1171,11 +1193,18 @@
         <f t="shared" si="2"/>
         <v>13.31230106544254</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>7.4454534926665816E-2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="G5" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.15000000000000002</v>
       </c>
       <c r="H5">
@@ -1193,8 +1222,15 @@
         <f t="shared" si="2"/>
         <v>13.04336959816381</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>7.5684627457998727E-2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1203,7 +1239,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="G6" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
       <c r="H6">
@@ -1221,8 +1257,12 @@
         <f t="shared" si="2"/>
         <v>12.774438130885081</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>7.6914719989331637E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1232,7 +1272,7 @@
         <v>60</v>
       </c>
       <c r="G7" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
       <c r="H7">
@@ -1250,8 +1290,12 @@
         <f t="shared" si="2"/>
         <v>12.505506663606351</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>7.8144812520664547E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1261,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
       <c r="H8">
@@ -1279,8 +1323,12 @@
         <f t="shared" si="2"/>
         <v>12.236575196327619</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>7.9374905051997457E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1298,7 +1346,7 @@
         <v>7.7737499999999988</v>
       </c>
       <c r="G9" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.35</v>
       </c>
       <c r="H9">
@@ -1316,8 +1364,12 @@
         <f t="shared" si="2"/>
         <v>11.96764372904889</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>8.0604997583330368E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1335,7 +1387,7 @@
         <v>0.70510204081632655</v>
       </c>
       <c r="G10" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.39999999999999997</v>
       </c>
       <c r="H10">
@@ -1353,8 +1405,12 @@
         <f t="shared" si="2"/>
         <v>11.698693390048657</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>8.1835176433917439E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
@@ -1372,7 +1428,7 @@
         <v>1.2948979591836736</v>
       </c>
       <c r="G11" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="H11">
@@ -1390,10 +1446,14 @@
         <f t="shared" si="2"/>
         <v>11.42978079449143</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>8.3065182645996188E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G12" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.49999999999999994</v>
       </c>
       <c r="H12">
@@ -1411,8 +1471,12 @@
         <f t="shared" si="2"/>
         <v>11.1608493272127</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>8.4295275177329099E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
@@ -1426,7 +1490,7 @@
         <v>29</v>
       </c>
       <c r="G13" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.54999999999999993</v>
       </c>
       <c r="H13">
@@ -1444,8 +1508,12 @@
         <f t="shared" si="2"/>
         <v>10.891917859933971</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>8.5525367708662009E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1457,7 +1525,7 @@
         <v>7.2201311118048853E-2</v>
       </c>
       <c r="G14" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.6</v>
       </c>
       <c r="H14">
@@ -1475,8 +1543,12 @@
         <f t="shared" si="2"/>
         <v>10.622986392655241</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>8.6755460239994919E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="G15" s="20">
@@ -1498,11 +1570,15 @@
         <f t="shared" si="2"/>
         <v>10.354054925376509</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>8.7985552771327843E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="G16" s="20">
-        <f t="shared" ref="G16:G22" si="4">G15+5%</f>
+        <f t="shared" ref="G16:G22" si="5">G15+5%</f>
         <v>0.70000000000000007</v>
       </c>
       <c r="H16">
@@ -1520,12 +1596,15 @@
         <f t="shared" si="2"/>
         <v>10.08512345809778</v>
       </c>
-      <c r="L16" s="21"/>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>8.921564530266074E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="G17" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.75000000000000011</v>
       </c>
       <c r="H17">
@@ -1543,10 +1622,14 @@
         <f t="shared" si="2"/>
         <v>9.8161919908190498</v>
       </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>9.044573783399365E-2</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G18" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.80000000000000016</v>
       </c>
       <c r="H18">
@@ -1564,10 +1647,14 @@
         <f t="shared" si="2"/>
         <v>9.5472605235403201</v>
       </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>9.167583036532656E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G19" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.8500000000000002</v>
       </c>
       <c r="H19">
@@ -1585,10 +1672,14 @@
         <f t="shared" si="2"/>
         <v>9.2783290562615903</v>
       </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>9.2905922896659471E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G20" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.90000000000000024</v>
       </c>
       <c r="H20">
@@ -1606,10 +1697,14 @@
         <f t="shared" si="2"/>
         <v>9.0093975889828606</v>
       </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>9.4136015427992381E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G21" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.95000000000000029</v>
       </c>
       <c r="H21">
@@ -1627,11 +1722,14 @@
         <f t="shared" si="2"/>
         <v>8.7404661217041308</v>
       </c>
-      <c r="L21" s="22"/>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>9.5366107959325291E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G22" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000002</v>
       </c>
       <c r="H22">
@@ -1648,6 +1746,10 @@
       <c r="K22">
         <f t="shared" si="2"/>
         <v>8.4809705151769084</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>9.6553040863580825E-2</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1660,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622EF6D1-D033-4A41-9B00-C212908A9BEE}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2010,8 +2112,630 @@
         <v>1.62015</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7.4</v>
+      </c>
+      <c r="B14">
+        <v>6.74</v>
+      </c>
+      <c r="C14">
+        <v>5.57</v>
+      </c>
+      <c r="D14">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E14">
+        <v>3.56</v>
+      </c>
+      <c r="F14">
+        <v>2.86</v>
+      </c>
+      <c r="G14">
+        <v>2.39</v>
+      </c>
+      <c r="H14">
+        <v>2.1</v>
+      </c>
+      <c r="I14">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6.59</v>
+      </c>
+      <c r="B15">
+        <v>5.98</v>
+      </c>
+      <c r="C15">
+        <v>5.48</v>
+      </c>
+      <c r="D15">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E15">
+        <v>3.56</v>
+      </c>
+      <c r="F15">
+        <v>2.86</v>
+      </c>
+      <c r="G15">
+        <v>2.39</v>
+      </c>
+      <c r="H15">
+        <v>2.1</v>
+      </c>
+      <c r="I15">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5.94</v>
+      </c>
+      <c r="B16">
+        <v>5.43</v>
+      </c>
+      <c r="C16">
+        <v>4.95</v>
+      </c>
+      <c r="D16">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E16">
+        <v>3.56</v>
+      </c>
+      <c r="F16">
+        <v>2.86</v>
+      </c>
+      <c r="G16">
+        <v>2.39</v>
+      </c>
+      <c r="H16">
+        <v>2.1</v>
+      </c>
+      <c r="I16">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5.45</v>
+      </c>
+      <c r="B17">
+        <v>4.96</v>
+      </c>
+      <c r="C17">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D17">
+        <v>4.3</v>
+      </c>
+      <c r="E17">
+        <v>3.56</v>
+      </c>
+      <c r="F17">
+        <v>2.86</v>
+      </c>
+      <c r="G17">
+        <v>2.39</v>
+      </c>
+      <c r="H17">
+        <v>2.1</v>
+      </c>
+      <c r="I17">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5.05</v>
+      </c>
+      <c r="B18">
+        <v>4.58</v>
+      </c>
+      <c r="C18">
+        <v>4.2</v>
+      </c>
+      <c r="D18">
+        <v>3.99</v>
+      </c>
+      <c r="E18">
+        <v>3.56</v>
+      </c>
+      <c r="F18">
+        <v>2.86</v>
+      </c>
+      <c r="G18">
+        <v>2.39</v>
+      </c>
+      <c r="H18">
+        <v>2.1</v>
+      </c>
+      <c r="I18">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4.72</v>
+      </c>
+      <c r="B19">
+        <v>4.3</v>
+      </c>
+      <c r="C19">
+        <v>3.94</v>
+      </c>
+      <c r="D19">
+        <v>3.71</v>
+      </c>
+      <c r="E19">
+        <v>3.54</v>
+      </c>
+      <c r="F19">
+        <v>2.86</v>
+      </c>
+      <c r="G19">
+        <v>2.39</v>
+      </c>
+      <c r="H19">
+        <v>2.1</v>
+      </c>
+      <c r="I19">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4.32</v>
+      </c>
+      <c r="B20">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="C20">
+        <v>3.68</v>
+      </c>
+      <c r="D20">
+        <v>3.48</v>
+      </c>
+      <c r="E20">
+        <v>3.31</v>
+      </c>
+      <c r="F20">
+        <v>2.86</v>
+      </c>
+      <c r="G20">
+        <v>2.39</v>
+      </c>
+      <c r="H20">
+        <v>2.1</v>
+      </c>
+      <c r="I20">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3.66</v>
+      </c>
+      <c r="B21">
+        <v>3.8</v>
+      </c>
+      <c r="C21">
+        <v>3.48</v>
+      </c>
+      <c r="D21">
+        <v>3.31</v>
+      </c>
+      <c r="E21">
+        <v>3.13</v>
+      </c>
+      <c r="F21">
+        <v>2.86</v>
+      </c>
+      <c r="G21">
+        <v>2.39</v>
+      </c>
+      <c r="H21">
+        <v>2.1</v>
+      </c>
+      <c r="I21">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3.17</v>
+      </c>
+      <c r="B22">
+        <v>3.51</v>
+      </c>
+      <c r="C22">
+        <v>3.29</v>
+      </c>
+      <c r="D22">
+        <v>3.13</v>
+      </c>
+      <c r="E22">
+        <v>2.98</v>
+      </c>
+      <c r="F22">
+        <v>2.71</v>
+      </c>
+      <c r="G22">
+        <v>2.39</v>
+      </c>
+      <c r="H22">
+        <v>2.1</v>
+      </c>
+      <c r="I22">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
+        <f>A14/'DWELL Stock'!A1</f>
+        <v>0.99972980275601186</v>
+      </c>
+      <c r="B26" s="20">
+        <f>B14/'DWELL Stock'!B1</f>
+        <v>1.1503669568185697</v>
+      </c>
+      <c r="C26" s="20">
+        <f>C14/'DWELL Stock'!C1</f>
+        <v>1.2001723766429648</v>
+      </c>
+      <c r="D26" s="20">
+        <f>D14/'DWELL Stock'!D1</f>
+        <v>1.2510785159620361</v>
+      </c>
+      <c r="E26" s="20">
+        <f>E14/'DWELL Stock'!E1</f>
+        <v>1.2801150665228336</v>
+      </c>
+      <c r="F26" s="20">
+        <f>F14/'DWELL Stock'!F1</f>
+        <v>1.2306368330464716</v>
+      </c>
+      <c r="G26" s="20">
+        <f>G14/'DWELL Stock'!G1</f>
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="H26" s="20">
+        <f>H14/'DWELL Stock'!H1</f>
+        <v>1.2082853855005755</v>
+      </c>
+      <c r="I26" s="20">
+        <f>I14/'DWELL Stock'!I1</f>
+        <v>1.1600777705767986</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
+        <f>A15/'DWELL Stock'!A2</f>
+        <v>0.9993933879284197</v>
+      </c>
+      <c r="B27" s="20">
+        <f>B15/'DWELL Stock'!B2</f>
+        <v>1.1493369210071114</v>
+      </c>
+      <c r="C27" s="20">
+        <f>C15/'DWELL Stock'!C2</f>
+        <v>1.200964277887355</v>
+      </c>
+      <c r="D27" s="20">
+        <f>D15/'DWELL Stock'!D2</f>
+        <v>1.2510785159620361</v>
+      </c>
+      <c r="E27" s="20">
+        <f>E15/'DWELL Stock'!E2</f>
+        <v>1.2801150665228336</v>
+      </c>
+      <c r="F27" s="20">
+        <f>F15/'DWELL Stock'!F2</f>
+        <v>1.2306368330464716</v>
+      </c>
+      <c r="G27" s="20">
+        <f>G15/'DWELL Stock'!G2</f>
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="H27" s="20">
+        <f>H15/'DWELL Stock'!H2</f>
+        <v>1.2082853855005755</v>
+      </c>
+      <c r="I27" s="20">
+        <f>I15/'DWELL Stock'!I2</f>
+        <v>1.1600777705767986</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
+        <f>A16/'DWELL Stock'!A3</f>
+        <v>1.0003368137420008</v>
+      </c>
+      <c r="B28" s="20">
+        <f>B16/'DWELL Stock'!B3</f>
+        <v>1.1506675143038778</v>
+      </c>
+      <c r="C28" s="20">
+        <f>C16/'DWELL Stock'!C3</f>
+        <v>1.2011647658335354</v>
+      </c>
+      <c r="D28" s="20">
+        <f>D16/'DWELL Stock'!D3</f>
+        <v>1.2510785159620361</v>
+      </c>
+      <c r="E28" s="20">
+        <f>E16/'DWELL Stock'!E3</f>
+        <v>1.2801150665228336</v>
+      </c>
+      <c r="F28" s="20">
+        <f>F16/'DWELL Stock'!F3</f>
+        <v>1.2306368330464716</v>
+      </c>
+      <c r="G28" s="20">
+        <f>G16/'DWELL Stock'!G3</f>
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="H28" s="20">
+        <f>H16/'DWELL Stock'!H3</f>
+        <v>1.2082853855005755</v>
+      </c>
+      <c r="I28" s="20">
+        <f>I16/'DWELL Stock'!I3</f>
+        <v>1.1600777705767986</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="20">
+        <f>A17/'DWELL Stock'!A4</f>
+        <v>1.0001835199119105</v>
+      </c>
+      <c r="B29" s="20">
+        <f>B17/'DWELL Stock'!B4</f>
+        <v>1.1492122335495829</v>
+      </c>
+      <c r="C29" s="20">
+        <f>C17/'DWELL Stock'!C4</f>
+        <v>1.1989389920424403</v>
+      </c>
+      <c r="D29" s="20">
+        <f>D17/'DWELL Stock'!D4</f>
+        <v>1.2507271669575333</v>
+      </c>
+      <c r="E29" s="20">
+        <f>E17/'DWELL Stock'!E4</f>
+        <v>1.2801150665228336</v>
+      </c>
+      <c r="F29" s="20">
+        <f>F17/'DWELL Stock'!F4</f>
+        <v>1.2306368330464716</v>
+      </c>
+      <c r="G29" s="20">
+        <f>G17/'DWELL Stock'!G4</f>
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="H29" s="20">
+        <f>H17/'DWELL Stock'!H4</f>
+        <v>1.2082853855005755</v>
+      </c>
+      <c r="I29" s="20">
+        <f>I17/'DWELL Stock'!I4</f>
+        <v>1.1600777705767986</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="20">
+        <f>A18/'DWELL Stock'!A5</f>
+        <v>1.0005944125222905</v>
+      </c>
+      <c r="B30" s="20">
+        <f>B18/'DWELL Stock'!B5</f>
+        <v>1.1495983935742973</v>
+      </c>
+      <c r="C30" s="20">
+        <f>C18/'DWELL Stock'!C5</f>
+        <v>1.2013729977116705</v>
+      </c>
+      <c r="D30" s="20">
+        <f>D18/'DWELL Stock'!D5</f>
+        <v>1.2488262910798122</v>
+      </c>
+      <c r="E30" s="20">
+        <f>E18/'DWELL Stock'!E5</f>
+        <v>1.2801150665228336</v>
+      </c>
+      <c r="F30" s="20">
+        <f>F18/'DWELL Stock'!F5</f>
+        <v>1.2306368330464716</v>
+      </c>
+      <c r="G30" s="20">
+        <f>G18/'DWELL Stock'!G5</f>
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="H30" s="20">
+        <f>H18/'DWELL Stock'!H5</f>
+        <v>1.2082853855005755</v>
+      </c>
+      <c r="I30" s="20">
+        <f>I18/'DWELL Stock'!I5</f>
+        <v>1.1600777705767986</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="20">
+        <f>A19/'DWELL Stock'!A6</f>
+        <v>1.0002119093028183</v>
+      </c>
+      <c r="B31" s="20">
+        <f>B19/'DWELL Stock'!B6</f>
+        <v>1.1491181186531265</v>
+      </c>
+      <c r="C31" s="20">
+        <f>C19/'DWELL Stock'!C6</f>
+        <v>1.2008533983541603</v>
+      </c>
+      <c r="D31" s="20">
+        <f>D19/'DWELL Stock'!D6</f>
+        <v>1.2495789828224992</v>
+      </c>
+      <c r="E31" s="20">
+        <f>E19/'DWELL Stock'!E6</f>
+        <v>1.2798264642082429</v>
+      </c>
+      <c r="F31" s="20">
+        <f>F19/'DWELL Stock'!F6</f>
+        <v>1.2306368330464716</v>
+      </c>
+      <c r="G31" s="20">
+        <f>G19/'DWELL Stock'!G6</f>
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="H31" s="20">
+        <f>H19/'DWELL Stock'!H6</f>
+        <v>1.2082853855005755</v>
+      </c>
+      <c r="I31" s="20">
+        <f>I19/'DWELL Stock'!I6</f>
+        <v>1.1600777705767986</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
+        <f>A20/'DWELL Stock'!A7</f>
+        <v>1.0009267840593143</v>
+      </c>
+      <c r="B32" s="20">
+        <f>B20/'DWELL Stock'!B7</f>
+        <v>1.1498855835240274</v>
+      </c>
+      <c r="C32" s="20">
+        <f>C20/'DWELL Stock'!C7</f>
+        <v>1.2002609262883237</v>
+      </c>
+      <c r="D32" s="20">
+        <f>D20/'DWELL Stock'!D7</f>
+        <v>1.2513484358144551</v>
+      </c>
+      <c r="E32" s="20">
+        <f>E20/'DWELL Stock'!E7</f>
+        <v>1.279969064191802</v>
+      </c>
+      <c r="F32" s="20">
+        <f>F20/'DWELL Stock'!F7</f>
+        <v>1.2306368330464716</v>
+      </c>
+      <c r="G32" s="20">
+        <f>G20/'DWELL Stock'!G7</f>
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="H32" s="20">
+        <f>H20/'DWELL Stock'!H7</f>
+        <v>1.2082853855005755</v>
+      </c>
+      <c r="I32" s="20">
+        <f>I20/'DWELL Stock'!I7</f>
+        <v>1.1600777705767986</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="20">
+        <f>A21/'DWELL Stock'!A8</f>
+        <v>0.99890829694323147</v>
+      </c>
+      <c r="B33" s="20">
+        <f>B21/'DWELL Stock'!B8</f>
+        <v>1.1511663132384125</v>
+      </c>
+      <c r="C33" s="20">
+        <f>C21/'DWELL Stock'!C8</f>
+        <v>1.2008281573498965</v>
+      </c>
+      <c r="D33" s="20">
+        <f>D21/'DWELL Stock'!D8</f>
+        <v>1.25</v>
+      </c>
+      <c r="E33" s="20">
+        <f>E21/'DWELL Stock'!E8</f>
+        <v>1.2822613682916837</v>
+      </c>
+      <c r="F33" s="20">
+        <f>F21/'DWELL Stock'!F8</f>
+        <v>1.2407809110629067</v>
+      </c>
+      <c r="G33" s="20">
+        <f>G21/'DWELL Stock'!G8</f>
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="H33" s="20">
+        <f>H21/'DWELL Stock'!H8</f>
+        <v>1.2082853855005755</v>
+      </c>
+      <c r="I33" s="20">
+        <f>I21/'DWELL Stock'!I8</f>
+        <v>1.1600777705767986</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="20">
+        <f>A22/'DWELL Stock'!A9</f>
+        <v>0.99936948297604034</v>
+      </c>
+      <c r="B34" s="20">
+        <f>B22/'DWELL Stock'!B9</f>
+        <v>1.1489361702127658</v>
+      </c>
+      <c r="C34" s="20">
+        <f>C22/'DWELL Stock'!C9</f>
+        <v>1.199854121079504</v>
+      </c>
+      <c r="D34" s="20">
+        <f>D22/'DWELL Stock'!D9</f>
+        <v>1.252</v>
+      </c>
+      <c r="E34" s="20">
+        <f>E22/'DWELL Stock'!E9</f>
+        <v>1.2822719449225475</v>
+      </c>
+      <c r="F34" s="20">
+        <f>F22/'DWELL Stock'!F9</f>
+        <v>1.2385740402193783</v>
+      </c>
+      <c r="G34" s="20">
+        <f>G22/'DWELL Stock'!G9</f>
+        <v>1.1997991967871486</v>
+      </c>
+      <c r="H34" s="20">
+        <f>H22/'DWELL Stock'!H9</f>
+        <v>1.2082853855005755</v>
+      </c>
+      <c r="I34" s="20">
+        <f>I22/'DWELL Stock'!I9</f>
+        <v>1.1600777705767986</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7403,6 +8127,534 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E88555-308C-4605-A6BF-A528911DB3A0}">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>13.85</v>
+      </c>
+      <c r="B2">
+        <f>A2/14.7</f>
+        <v>0.94217687074829937</v>
+      </c>
+      <c r="C2">
+        <v>7.1959999999999996E-2</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE("f(",B2,")=",C2)</f>
+        <v>f(0.942176870748299)=0.07196</v>
+      </c>
+      <c r="G2">
+        <f>(0.018604117/-0.273469387755102)*B2+0.136058</f>
+        <v>7.1961726256218897E-2</v>
+      </c>
+      <c r="H2">
+        <f>-0.067777*B2+0.135743</f>
+        <v>7.1885078231292518E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9.83</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B36" si="0">A3/14.7</f>
+        <v>0.66870748299319727</v>
+      </c>
+      <c r="C3">
+        <v>9.0564117E-2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D4" si="1">CONCATENATE("f(",B3,")=",C3)</f>
+        <v>f(0.668707482993197)=0.090564117</v>
+      </c>
+      <c r="G3">
+        <f>(0.018604117/-0.273469387755102)*B3+0.136058</f>
+        <v>9.0565843256218914E-2</v>
+      </c>
+      <c r="H3">
+        <f>-0.067777*B3+0.135743</f>
+        <v>9.0420012925170073E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.59863945578231303</v>
+      </c>
+      <c r="C4">
+        <v>9.4951174999999999E-2</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>f(0.598639455782313)=0.094951175</v>
+      </c>
+      <c r="G4">
+        <f>(0.018604117/-0.273469387755102)*B4+0.136058</f>
+        <v>9.5332569751243781E-2</v>
+      </c>
+      <c r="H4">
+        <f>-0.067777*B4+0.135743</f>
+        <v>9.5169013605442165E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.68027210884353739</v>
+      </c>
+      <c r="H6">
+        <f>-0.067777*B6+0.135743</f>
+        <v>8.9636197278911561E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>A6-0.1</f>
+        <v>9.9</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0.67346938775510212</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H36" si="2">-0.067777*B7+0.135743</f>
+        <v>9.0097265306122443E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" ref="A8:A36" si="3">A7-0.1</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>9.0558333333333324E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="3"/>
+        <v>9.7000000000000011</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>0.65986394557823136</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>9.1019401360544205E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="3"/>
+        <v>9.6000000000000014</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>0.65306122448979609</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>9.1480469387755087E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>9.5000000000000018</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>0.64625850340136071</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>9.1941537414965968E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="3"/>
+        <v>9.4000000000000021</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0.63945578231292532</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>9.2402605442176863E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>9.3000000000000025</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>0.63265306122448994</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>9.2863673469387745E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>9.2000000000000028</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0.62585034013605467</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>9.3324741496598612E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="3"/>
+        <v>9.1000000000000032</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0.61904761904761929</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>9.3785809523809507E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="3"/>
+        <v>9.0000000000000036</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0.61224489795918391</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>9.4246877551020403E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="3"/>
+        <v>8.9000000000000039</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0.60544217687074864</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>9.470794557823127E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>8.8000000000000043</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.59863945578231326</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>9.5169013605442151E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>8.7000000000000046</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0.59183673469387788</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>9.5630081632653047E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>8.600000000000005</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.58503401360544249</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>9.6091149659863928E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>8.5000000000000053</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.57823129251700722</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>9.6552217687074809E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="3"/>
+        <v>8.4000000000000057</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>0.57142857142857184</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>9.7013285714285691E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="3"/>
+        <v>8.300000000000006</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0.56462585034013646</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>9.7474353741496572E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="3"/>
+        <v>8.2000000000000064</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>0.55782312925170119</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>9.7935421768707454E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="3"/>
+        <v>8.1000000000000068</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>0.55102040816326581</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>9.8396489795918335E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="3"/>
+        <v>8.0000000000000071</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>0.54421768707483043</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>9.8857557823129216E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="3"/>
+        <v>7.9000000000000075</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>0.53741496598639504</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>9.9318625850340098E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="3"/>
+        <v>7.8000000000000078</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0.53061224489795977</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>9.9779693877550979E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="3"/>
+        <v>7.7000000000000082</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0.52380952380952439</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>0.10024076190476186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="3"/>
+        <v>7.6000000000000085</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>0.51700680272108901</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>0.10070182993197274</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="3"/>
+        <v>7.5000000000000089</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>0.51020408163265374</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>0.10116289795918362</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="3"/>
+        <v>7.4000000000000092</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>0.50340136054421836</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>0.1016239659863945</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="3"/>
+        <v>7.3000000000000096</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0.49659863945578298</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>0.1020850340136054</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="3"/>
+        <v>7.2000000000000099</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>0.48979591836734765</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>0.10254610204081628</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="3"/>
+        <v>7.1000000000000103</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>0.48299319727891227</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>0.10300717006802716</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="3"/>
+        <v>7.0000000000000107</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>0.47619047619047694</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>0.10346823809523804</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B0A50C-E886-462D-8E67-A0D9190AD867}">
   <dimension ref="A1:H72"/>
@@ -7414,7 +8666,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B1" t="s">
@@ -7425,7 +8677,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="23">
+      <c r="A2" s="21">
         <v>0.5</v>
       </c>
       <c r="B2">
@@ -7436,7 +8688,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
+      <c r="A3" s="21">
         <v>0.51</v>
       </c>
       <c r="B3">
@@ -7447,7 +8699,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="21">
         <v>0.52</v>
       </c>
       <c r="B4">
@@ -7458,7 +8710,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="21">
         <v>0.53</v>
       </c>
       <c r="B5">
@@ -7469,7 +8721,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="21">
         <v>0.54</v>
       </c>
       <c r="B6">
@@ -7480,7 +8732,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="21">
         <v>0.55000000000000004</v>
       </c>
       <c r="B7">
@@ -7491,7 +8743,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="21">
         <v>0.56000000000000005</v>
       </c>
       <c r="B8">
@@ -7502,7 +8754,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
+      <c r="A9" s="21">
         <v>0.56999999999999995</v>
       </c>
       <c r="B9">
@@ -7513,7 +8765,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="21">
         <v>0.57999999999999996</v>
       </c>
       <c r="B10">
@@ -7524,7 +8776,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="21">
         <v>0.59</v>
       </c>
       <c r="B11">
@@ -7535,7 +8787,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="21">
         <v>0.6</v>
       </c>
       <c r="B12">
@@ -7546,7 +8798,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="21">
         <v>0.61</v>
       </c>
       <c r="B13">
@@ -7557,7 +8809,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="23">
+      <c r="A14" s="21">
         <v>0.62</v>
       </c>
       <c r="B14">
@@ -7568,7 +8820,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
+      <c r="A15" s="21">
         <v>0.63</v>
       </c>
       <c r="B15">
@@ -7579,7 +8831,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
+      <c r="A16" s="21">
         <v>0.64</v>
       </c>
       <c r="B16">
@@ -7590,7 +8842,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="23">
+      <c r="A17" s="21">
         <v>0.65</v>
       </c>
       <c r="B17">
@@ -7601,7 +8853,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="23">
+      <c r="A18" s="21">
         <v>0.66</v>
       </c>
       <c r="B18">
@@ -7612,7 +8864,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="23">
+      <c r="A19" s="21">
         <v>0.67</v>
       </c>
       <c r="B19">
@@ -7623,7 +8875,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="23">
+      <c r="A20" s="21">
         <v>0.68</v>
       </c>
       <c r="B20">
@@ -7634,7 +8886,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="23">
+      <c r="A21" s="21">
         <v>0.69</v>
       </c>
       <c r="B21">
@@ -7645,7 +8897,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="23">
+      <c r="A22" s="21">
         <v>0.7</v>
       </c>
       <c r="B22">
@@ -7656,7 +8908,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="23">
+      <c r="A23" s="21">
         <v>0.71</v>
       </c>
       <c r="B23">
@@ -7667,7 +8919,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="23">
+      <c r="A24" s="21">
         <v>0.72</v>
       </c>
       <c r="B24">
@@ -7678,7 +8930,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="23">
+      <c r="A25" s="21">
         <v>0.73</v>
       </c>
       <c r="B25">
@@ -7704,7 +8956,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="23">
+      <c r="A26" s="21">
         <v>0.74</v>
       </c>
       <c r="B26">
@@ -7715,7 +8967,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
+      <c r="A27" s="21">
         <v>0.75</v>
       </c>
       <c r="B27">
@@ -7732,7 +8984,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
+      <c r="A28" s="21">
         <v>0.76</v>
       </c>
       <c r="B28">
@@ -7743,7 +8995,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="23">
+      <c r="A29" s="21">
         <v>0.77</v>
       </c>
       <c r="B29">
@@ -7766,7 +9018,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="23">
+      <c r="A30" s="21">
         <v>0.78</v>
       </c>
       <c r="B30">
@@ -7777,7 +9029,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="23">
+      <c r="A31" s="21">
         <v>0.79</v>
       </c>
       <c r="B31">
@@ -7788,7 +9040,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="23">
+      <c r="A32" s="21">
         <v>0.8</v>
       </c>
       <c r="B32">
@@ -7808,7 +9060,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="23">
+      <c r="A33" s="21">
         <v>0.81</v>
       </c>
       <c r="B33">
@@ -7819,7 +9071,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="23">
+      <c r="A34" s="21">
         <v>0.82</v>
       </c>
       <c r="B34">
@@ -7830,7 +9082,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="23">
+      <c r="A35" s="21">
         <v>0.83</v>
       </c>
       <c r="B35">
@@ -7841,7 +9093,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="23">
+      <c r="A36" s="21">
         <v>0.84</v>
       </c>
       <c r="B36">
@@ -7864,7 +9116,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="23">
+      <c r="A37" s="21">
         <v>0.85</v>
       </c>
       <c r="B37">
@@ -7875,7 +9127,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="23">
+      <c r="A38" s="21">
         <v>0.86</v>
       </c>
       <c r="B38">
@@ -7886,7 +9138,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="23">
+      <c r="A39" s="21">
         <v>0.87</v>
       </c>
       <c r="B39">
@@ -7903,7 +9155,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="23">
+      <c r="A40" s="21">
         <v>0.88</v>
       </c>
       <c r="B40">
@@ -7914,7 +9166,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="23">
+      <c r="A41" s="21">
         <v>0.89</v>
       </c>
       <c r="B41">
@@ -7925,7 +9177,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="23">
+      <c r="A42" s="21">
         <v>0.9</v>
       </c>
       <c r="B42">
@@ -7936,7 +9188,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="23">
+      <c r="A43" s="21">
         <v>0.91</v>
       </c>
       <c r="B43">
@@ -7962,7 +9214,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="23">
+      <c r="A44" s="21">
         <v>0.92</v>
       </c>
       <c r="B44">
@@ -7973,7 +9225,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="23">
+      <c r="A45" s="21">
         <v>0.93</v>
       </c>
       <c r="B45">
@@ -7984,7 +9236,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="23">
+      <c r="A46" s="21">
         <v>0.94</v>
       </c>
       <c r="B46">
@@ -7995,7 +9247,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="23">
+      <c r="A47" s="21">
         <v>0.95</v>
       </c>
       <c r="B47">
@@ -8006,7 +9258,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="23">
+      <c r="A48" s="21">
         <v>0.96</v>
       </c>
       <c r="B48">
@@ -8017,7 +9269,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="23">
+      <c r="A49" s="21">
         <v>0.97</v>
       </c>
       <c r="B49">
@@ -8028,7 +9280,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="23">
+      <c r="A50" s="21">
         <v>0.98</v>
       </c>
       <c r="B50">
@@ -8039,7 +9291,7 @@
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="23">
+      <c r="A51" s="21">
         <v>0.99</v>
       </c>
       <c r="B51">
@@ -8050,7 +9302,7 @@
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="23">
+      <c r="A52" s="21">
         <v>1</v>
       </c>
       <c r="B52">
@@ -8061,7 +9313,7 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="23">
+      <c r="A53" s="21">
         <v>1.01</v>
       </c>
       <c r="B53">
@@ -8072,7 +9324,7 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="23">
+      <c r="A54" s="21">
         <v>1.02</v>
       </c>
       <c r="B54">
@@ -8083,7 +9335,7 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="23">
+      <c r="A55" s="21">
         <v>1.03</v>
       </c>
       <c r="B55">
@@ -8094,7 +9346,7 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="23">
+      <c r="A56" s="21">
         <v>1.04</v>
       </c>
       <c r="B56">
@@ -8105,7 +9357,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="23">
+      <c r="A57" s="21">
         <v>1.05</v>
       </c>
       <c r="B57">
@@ -8116,7 +9368,7 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="23">
+      <c r="A58" s="21">
         <v>1.06</v>
       </c>
       <c r="B58">
@@ -8127,7 +9379,7 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="23">
+      <c r="A59" s="21">
         <v>1.07</v>
       </c>
       <c r="B59">
@@ -8138,7 +9390,7 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="23">
+      <c r="A60" s="21">
         <v>1.08</v>
       </c>
       <c r="B60">
@@ -8149,7 +9401,7 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="23">
+      <c r="A61" s="21">
         <v>1.0900000000000001</v>
       </c>
       <c r="B61">
@@ -8160,7 +9412,7 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="23">
+      <c r="A62" s="21">
         <v>1.1000000000000001</v>
       </c>
       <c r="B62">
@@ -8171,7 +9423,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="23">
+      <c r="A63" s="21">
         <v>1.1100000000000001</v>
       </c>
       <c r="B63">
@@ -8182,7 +9434,7 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="23">
+      <c r="A64" s="21">
         <v>1.1200000000000001</v>
       </c>
       <c r="B64">
@@ -8193,7 +9445,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="23">
+      <c r="A65" s="21">
         <v>1.1299999999999999</v>
       </c>
       <c r="B65">
@@ -8204,7 +9456,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="23">
+      <c r="A66" s="21">
         <v>1.1399999999999999</v>
       </c>
       <c r="B66">
@@ -8215,7 +9467,7 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="23">
+      <c r="A67" s="21">
         <v>1.1499999999999999</v>
       </c>
       <c r="B67">
@@ -8226,7 +9478,7 @@
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="23">
+      <c r="A68" s="21">
         <v>1.1599999999999999</v>
       </c>
       <c r="B68">
@@ -8237,7 +9489,7 @@
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="23">
+      <c r="A69" s="21">
         <v>1.17</v>
       </c>
       <c r="B69">
@@ -8248,7 +9500,7 @@
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="23">
+      <c r="A70" s="21">
         <v>1.18</v>
       </c>
       <c r="B70">
@@ -8259,7 +9511,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="23">
+      <c r="A71" s="21">
         <v>1.19</v>
       </c>
       <c r="B71">
@@ -8270,7 +9522,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="23">
+      <c r="A72" s="21">
         <v>1.2</v>
       </c>
       <c r="B72">
@@ -13986,7 +15238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC026DA-F509-4385-B6B3-72E60872EBDC}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18:G18"/>
     </sheetView>
   </sheetViews>
@@ -14214,63 +15466,63 @@
       <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="22">
         <f>B2+30%*B2</f>
         <v>132.34</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="22">
         <f t="shared" ref="C5:P5" si="1">C2+30%*C2</f>
         <v>79.091999999999999</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="22">
         <f t="shared" si="1"/>
         <v>45.5</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="22">
         <f t="shared" si="1"/>
         <v>45.5</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="22">
         <f t="shared" si="1"/>
         <v>45.5</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="22">
         <f t="shared" si="1"/>
         <v>45.5</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="22">
         <f t="shared" si="1"/>
         <v>45.5</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="22">
         <f t="shared" si="1"/>
         <v>45.5</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="22">
         <f t="shared" si="1"/>
         <v>45.5</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="22">
         <f t="shared" si="1"/>
         <v>11.7</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="22">
         <f t="shared" si="1"/>
         <v>10.4</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="22">
         <f t="shared" si="1"/>
         <v>6.8224</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="22">
         <f t="shared" si="1"/>
         <v>4.0872000000000002</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="22">
         <f t="shared" si="1"/>
         <v>4.0872000000000002</v>
       </c>
-      <c r="P5" s="24">
+      <c r="P5" s="22">
         <f t="shared" si="1"/>
         <v>4.0872000000000002</v>
       </c>
@@ -14763,8 +16015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745AD7B9-4B1D-4E8C-A42C-E86EAA5F24F9}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>